<commit_message>
Testing on the way
</commit_message>
<xml_diff>
--- a/Test.xlsx
+++ b/Test.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="10">
   <si>
     <t>f(x,y)=x+y</t>
   </si>
@@ -34,6 +34,18 @@
   </si>
   <si>
     <t>Platform</t>
+  </si>
+  <si>
+    <t>f(x)=x</t>
+  </si>
+  <si>
+    <t>PASS</t>
+  </si>
+  <si>
+    <t>f(x)=x+12+sin(b)</t>
+  </si>
+  <si>
+    <t>FAILED</t>
   </si>
 </sst>
 </file>
@@ -365,15 +377,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.42578125" customWidth="1"/>
+    <col min="5" max="5" width="14.140625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -387,7 +404,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:6">
       <c r="A2">
         <v>1</v>
       </c>
@@ -396,6 +413,37 @@
       </c>
       <c r="D2" t="s">
         <v>2</v>
+      </c>
+      <c r="F2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" t="s">
+        <v>2</v>
+      </c>
+      <c r="F4" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
get back to nlabparser
</commit_message>
<xml_diff>
--- a/Test.xlsx
+++ b/Test.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="20055" windowHeight="7935"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="19440" windowHeight="7935"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="17">
   <si>
     <t>f(x,y)=x+y</t>
   </si>
@@ -46,13 +46,34 @@
   </si>
   <si>
     <t>FAILED</t>
+  </si>
+  <si>
+    <t>f(x,y)=sin(x)+cos(y)</t>
+  </si>
+  <si>
+    <t>CRITICAL</t>
+  </si>
+  <si>
+    <t>SEVERE</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>f(x,y)=sin((x+cos(y)))</t>
+  </si>
+  <si>
+    <t>Hint</t>
+  </si>
+  <si>
+    <t>analyse the output tree</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -89,6 +110,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -167,6 +193,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -201,6 +228,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -376,21 +404,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.42578125" customWidth="1"/>
     <col min="5" max="5" width="14.140625" customWidth="1"/>
+    <col min="7" max="7" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -403,8 +433,17 @@
       <c r="D1" t="s">
         <v>5</v>
       </c>
+      <c r="E1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H1" t="s">
+        <v>15</v>
+      </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -418,7 +457,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -432,7 +471,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -442,8 +481,34 @@
       <c r="D4" t="s">
         <v>2</v>
       </c>
+      <c r="E4" t="s">
+        <v>11</v>
+      </c>
       <c r="F4" t="s">
         <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H5" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -452,24 +517,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
criteria on the way
</commit_message>
<xml_diff>
--- a/Test.xlsx
+++ b/Test.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="19440" windowHeight="7935"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="19440" windowHeight="7935" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Time" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="24">
   <si>
     <t>f(x,y)=x+y</t>
   </si>
@@ -67,13 +67,34 @@
   </si>
   <si>
     <t>analyse the output tree</t>
+  </si>
+  <si>
+    <t>Project</t>
+  </si>
+  <si>
+    <t>Time</t>
+  </si>
+  <si>
+    <t>LIBNMATH</t>
+  </si>
+  <si>
+    <t>1h</t>
+  </si>
+  <si>
+    <t>1d</t>
+  </si>
+  <si>
+    <t>FunctionPlotter</t>
+  </si>
+  <si>
+    <t>USD</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -82,12 +103,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -102,8 +129,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="15" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -193,7 +223,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -228,7 +257,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -404,14 +432,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="18.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.42578125" customWidth="1"/>
@@ -420,7 +448,7 @@
     <col min="8" max="8" width="16.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -443,7 +471,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8">
       <c r="A2">
         <v>1</v>
       </c>
@@ -457,7 +485,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8">
       <c r="A3">
         <v>2</v>
       </c>
@@ -471,7 +499,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8">
       <c r="A4">
         <v>3</v>
       </c>
@@ -488,7 +516,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8">
       <c r="A5">
         <v>4</v>
       </c>
@@ -517,24 +545,195 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:J26"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="13.140625" customWidth="1"/>
+    <col min="2" max="2" width="13.85546875" customWidth="1"/>
+    <col min="3" max="3" width="10.42578125" customWidth="1"/>
+    <col min="4" max="5" width="11.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2" s="1">
+        <v>41815</v>
+      </c>
+      <c r="C2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3" s="1">
+        <v>41816</v>
+      </c>
+      <c r="C3">
+        <v>3</v>
+      </c>
+      <c r="I3">
+        <v>21</v>
+      </c>
+      <c r="J3">
+        <v>780</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4" s="1">
+        <v>41817</v>
+      </c>
+      <c r="C4">
+        <v>3</v>
+      </c>
+      <c r="I4" t="s">
+        <v>21</v>
+      </c>
+      <c r="J4">
+        <f>J3/I3</f>
+        <v>37.142857142857146</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5" s="2">
+        <v>41818</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" s="3">
+        <v>8</v>
+      </c>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" t="s">
+        <v>20</v>
+      </c>
+      <c r="J5">
+        <f>J4/8</f>
+        <v>4.6428571428571432</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6" s="2">
+        <v>41819</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" s="3">
+        <v>8</v>
+      </c>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" t="s">
+        <v>23</v>
+      </c>
+      <c r="J6">
+        <v>21390</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7" s="1">
+        <v>41820</v>
+      </c>
+      <c r="B7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="A8" s="1">
+        <v>41821</v>
+      </c>
+      <c r="B8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
+      <c r="A9" s="1">
+        <v>41822</v>
+      </c>
+      <c r="B9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
+      <c r="A10" s="1">
+        <v>41823</v>
+      </c>
+      <c r="B10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
+      <c r="A11" s="1">
+        <v>41824</v>
+      </c>
+      <c r="B11" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="26" spans="3:5">
+      <c r="C26">
+        <f>SUM(C2:C25)</f>
+        <v>48</v>
+      </c>
+      <c r="D26">
+        <f>C26*J5</f>
+        <v>222.85714285714289</v>
+      </c>
+      <c r="E26">
+        <f>D26*J6</f>
+        <v>4766914.2857142864</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Fixed criteria for SIMPLE & COMBINED
</commit_message>
<xml_diff>
--- a/Test.xlsx
+++ b/Test.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="19440" windowHeight="7935"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="19440" windowHeight="7935" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Testcases" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="37">
   <si>
     <t>f(x,y)=x+y</t>
   </si>
@@ -493,8 +493,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -622,7 +622,7 @@
         <v>11</v>
       </c>
       <c r="F7" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -632,10 +632,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H68"/>
+  <dimension ref="A1:H69"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="G75" sqref="G75"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C70" sqref="C70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -676,15 +676,15 @@
       </c>
       <c r="F2">
         <f>SUM(C4:C9878)</f>
-        <v>207</v>
+        <v>213</v>
       </c>
       <c r="G2">
         <f>SUM($C$4:$C$204)*$B$2</f>
-        <v>952.19999999999993</v>
+        <v>979.8</v>
       </c>
       <c r="H2">
         <f>$G$2*$D$2</f>
-        <v>20367558</v>
+        <v>20957922</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -1397,6 +1397,17 @@
       </c>
       <c r="C68">
         <v>8</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69" s="1">
+        <v>41856</v>
+      </c>
+      <c r="B69" t="s">
+        <v>16</v>
+      </c>
+      <c r="C69">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
turn parseFunctionExpression to public
</commit_message>
<xml_diff>
--- a/Test.xlsx
+++ b/Test.xlsx
@@ -10,13 +10,14 @@
     <sheet name="Testcases" sheetId="1" r:id="rId1"/>
     <sheet name="Time" sheetId="2" r:id="rId2"/>
     <sheet name="Tasks" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="47">
   <si>
     <t>f(x,y)=x+y</t>
   </si>
@@ -136,6 +137,27 @@
   </si>
   <si>
     <t>Completed</t>
+  </si>
+  <si>
+    <t>SUN</t>
+  </si>
+  <si>
+    <t>MON</t>
+  </si>
+  <si>
+    <t>TUE</t>
+  </si>
+  <si>
+    <t>WED</t>
+  </si>
+  <si>
+    <t>THU</t>
+  </si>
+  <si>
+    <t>FRI</t>
+  </si>
+  <si>
+    <t>SAT</t>
   </si>
 </sst>
 </file>
@@ -191,7 +213,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="15" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
@@ -199,6 +221,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="15" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -503,7 +528,7 @@
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="D10" sqref="C10:D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -641,815 +666,1573 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H72"/>
+  <dimension ref="A1:I112"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="C73" sqref="C73"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="D113" sqref="D113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.140625" customWidth="1"/>
-    <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.42578125" customWidth="1"/>
-    <col min="4" max="5" width="11.140625" customWidth="1"/>
-    <col min="7" max="7" width="13.85546875" customWidth="1"/>
+    <col min="2" max="2" width="13.140625" style="7" customWidth="1"/>
+    <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.42578125" customWidth="1"/>
+    <col min="5" max="6" width="11.140625" customWidth="1"/>
+    <col min="8" max="8" width="13.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="F1" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G1" t="s">
         <v>20</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>22</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="4">
+      <c r="C2" s="4">
         <v>4.5999999999999996</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>19</v>
       </c>
-      <c r="D2" s="4">
+      <c r="E2" s="4">
         <v>21390</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>21</v>
       </c>
-      <c r="F2">
-        <f>SUM(C4:C9878)</f>
-        <v>233</v>
-      </c>
       <c r="G2">
-        <f>SUM($C$4:$C$204)*$B$2</f>
-        <v>1071.8</v>
+        <f>SUM(D4:D9878)</f>
+        <v>398</v>
       </c>
       <c r="H2">
-        <f>$G$2*$D$2</f>
-        <v>22925802</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+        <f>SUM($D$4:$D$204)*$C$2</f>
+        <v>1830.8</v>
+      </c>
+      <c r="I2">
+        <f>$H$2*$E$2</f>
+        <v>39160812</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="8"/>
+      <c r="C3" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="D3" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D3" s="4"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E3" s="4"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
         <v>41790</v>
       </c>
-      <c r="B4" s="6"/>
-      <c r="C4" s="6">
-        <v>2</v>
-      </c>
-      <c r="D4" s="6"/>
+      <c r="B4" s="9" t="str">
+        <f>HLOOKUP(WEEKDAY(A4),Sheet1!$A$1:$G$2,2,FALSE)</f>
+        <v>SAT</v>
+      </c>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6">
+        <v>2</v>
+      </c>
       <c r="E4" s="6"/>
       <c r="F4" s="6"/>
       <c r="G4" s="6"/>
       <c r="H4" s="6"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I4" s="6"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
         <v>41791</v>
       </c>
-      <c r="B5" s="6"/>
-      <c r="C5" s="6">
-        <v>2</v>
-      </c>
-      <c r="D5" s="6"/>
+      <c r="B5" s="9" t="str">
+        <f>HLOOKUP(WEEKDAY(A5),Sheet1!$A$1:$G$2,2,FALSE)</f>
+        <v>SUN</v>
+      </c>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6">
+        <v>2</v>
+      </c>
       <c r="E5" s="6"/>
       <c r="F5" s="6"/>
       <c r="G5" s="6"/>
       <c r="H5" s="6"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I5" s="6"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>41792</v>
       </c>
-      <c r="C6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B6" s="9" t="str">
+        <f>HLOOKUP(WEEKDAY(A6),Sheet1!$A$1:$G$2,2,FALSE)</f>
+        <v>MON</v>
+      </c>
+      <c r="D6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>41793</v>
       </c>
-      <c r="C7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B7" s="9" t="str">
+        <f>HLOOKUP(WEEKDAY(A7),Sheet1!$A$1:$G$2,2,FALSE)</f>
+        <v>TUE</v>
+      </c>
+      <c r="D7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>41794</v>
       </c>
-      <c r="C8">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B8" s="9" t="str">
+        <f>HLOOKUP(WEEKDAY(A8),Sheet1!$A$1:$G$2,2,FALSE)</f>
+        <v>WED</v>
+      </c>
+      <c r="D8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>41795</v>
       </c>
-      <c r="C9">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B9" s="9" t="str">
+        <f>HLOOKUP(WEEKDAY(A9),Sheet1!$A$1:$G$2,2,FALSE)</f>
+        <v>THU</v>
+      </c>
+      <c r="D9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>41796</v>
       </c>
-      <c r="C10">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B10" s="9" t="str">
+        <f>HLOOKUP(WEEKDAY(A10),Sheet1!$A$1:$G$2,2,FALSE)</f>
+        <v>FRI</v>
+      </c>
+      <c r="D10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
         <v>41797</v>
       </c>
-      <c r="B11" s="6"/>
-      <c r="C11" s="6">
-        <v>2</v>
-      </c>
-      <c r="D11" s="6"/>
+      <c r="B11" s="9" t="str">
+        <f>HLOOKUP(WEEKDAY(A11),Sheet1!$A$1:$G$2,2,FALSE)</f>
+        <v>SAT</v>
+      </c>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6">
+        <v>2</v>
+      </c>
       <c r="E11" s="6"/>
       <c r="F11" s="6"/>
       <c r="G11" s="6"/>
       <c r="H11" s="6"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I11" s="6"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
         <v>41798</v>
       </c>
-      <c r="B12" s="6"/>
-      <c r="C12" s="6">
+      <c r="B12" s="9" t="str">
+        <f>HLOOKUP(WEEKDAY(A12),Sheet1!$A$1:$G$2,2,FALSE)</f>
+        <v>SUN</v>
+      </c>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6">
         <v>6</v>
       </c>
-      <c r="D12" s="6"/>
       <c r="E12" s="6"/>
       <c r="F12" s="6"/>
       <c r="G12" s="6"/>
       <c r="H12" s="6"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I12" s="6"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>41799</v>
       </c>
-      <c r="C13">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B13" s="9" t="str">
+        <f>HLOOKUP(WEEKDAY(A13),Sheet1!$A$1:$G$2,2,FALSE)</f>
+        <v>MON</v>
+      </c>
+      <c r="D13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>41800</v>
       </c>
-      <c r="C14">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B14" s="9" t="str">
+        <f>HLOOKUP(WEEKDAY(A14),Sheet1!$A$1:$G$2,2,FALSE)</f>
+        <v>TUE</v>
+      </c>
+      <c r="D14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>41801</v>
       </c>
-      <c r="C15">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B15" s="9" t="str">
+        <f>HLOOKUP(WEEKDAY(A15),Sheet1!$A$1:$G$2,2,FALSE)</f>
+        <v>WED</v>
+      </c>
+      <c r="D15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>41802</v>
       </c>
-      <c r="C16">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B16" s="9" t="str">
+        <f>HLOOKUP(WEEKDAY(A16),Sheet1!$A$1:$G$2,2,FALSE)</f>
+        <v>THU</v>
+      </c>
+      <c r="D16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>41803</v>
       </c>
-      <c r="C17">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B17" s="9" t="str">
+        <f>HLOOKUP(WEEKDAY(A17),Sheet1!$A$1:$G$2,2,FALSE)</f>
+        <v>FRI</v>
+      </c>
+      <c r="D17">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
         <v>41804</v>
       </c>
-      <c r="B18" s="6"/>
-      <c r="C18" s="6">
-        <v>2</v>
-      </c>
-      <c r="D18" s="6"/>
+      <c r="B18" s="9" t="str">
+        <f>HLOOKUP(WEEKDAY(A18),Sheet1!$A$1:$G$2,2,FALSE)</f>
+        <v>SAT</v>
+      </c>
+      <c r="C18" s="6"/>
+      <c r="D18" s="6">
+        <v>2</v>
+      </c>
       <c r="E18" s="6"/>
       <c r="F18" s="6"/>
       <c r="G18" s="6"/>
       <c r="H18" s="6"/>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I18" s="6"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="5">
         <v>41805</v>
       </c>
-      <c r="B19" s="6"/>
-      <c r="C19" s="6">
+      <c r="B19" s="9" t="str">
+        <f>HLOOKUP(WEEKDAY(A19),Sheet1!$A$1:$G$2,2,FALSE)</f>
+        <v>SUN</v>
+      </c>
+      <c r="C19" s="6"/>
+      <c r="D19" s="6">
         <v>4</v>
       </c>
-      <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
       <c r="H19" s="6"/>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I19" s="6"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>41806</v>
       </c>
-      <c r="C20">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B20" s="9" t="str">
+        <f>HLOOKUP(WEEKDAY(A20),Sheet1!$A$1:$G$2,2,FALSE)</f>
+        <v>MON</v>
+      </c>
+      <c r="D20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>41807</v>
       </c>
-      <c r="C21">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B21" s="9" t="str">
+        <f>HLOOKUP(WEEKDAY(A21),Sheet1!$A$1:$G$2,2,FALSE)</f>
+        <v>TUE</v>
+      </c>
+      <c r="D21">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>41808</v>
       </c>
-      <c r="C22">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B22" s="9" t="str">
+        <f>HLOOKUP(WEEKDAY(A22),Sheet1!$A$1:$G$2,2,FALSE)</f>
+        <v>WED</v>
+      </c>
+      <c r="D22">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>41809</v>
       </c>
-      <c r="C23">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B23" s="9" t="str">
+        <f>HLOOKUP(WEEKDAY(A23),Sheet1!$A$1:$G$2,2,FALSE)</f>
+        <v>THU</v>
+      </c>
+      <c r="D23">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>41810</v>
       </c>
-      <c r="C24">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B24" s="9" t="str">
+        <f>HLOOKUP(WEEKDAY(A24),Sheet1!$A$1:$G$2,2,FALSE)</f>
+        <v>FRI</v>
+      </c>
+      <c r="D24">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="5">
         <v>41811</v>
       </c>
-      <c r="B25" s="6"/>
-      <c r="C25" s="6">
+      <c r="B25" s="9" t="str">
+        <f>HLOOKUP(WEEKDAY(A25),Sheet1!$A$1:$G$2,2,FALSE)</f>
+        <v>SAT</v>
+      </c>
+      <c r="C25" s="6"/>
+      <c r="D25" s="6">
         <v>8</v>
       </c>
-      <c r="D25" s="6"/>
       <c r="E25" s="6"/>
       <c r="F25" s="6"/>
       <c r="G25" s="6"/>
       <c r="H25" s="6"/>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I25" s="6"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="5">
         <v>41812</v>
       </c>
-      <c r="B26" s="6"/>
-      <c r="C26" s="6">
+      <c r="B26" s="9" t="str">
+        <f>HLOOKUP(WEEKDAY(A26),Sheet1!$A$1:$G$2,2,FALSE)</f>
+        <v>SUN</v>
+      </c>
+      <c r="C26" s="6"/>
+      <c r="D26" s="6">
         <v>8</v>
       </c>
-      <c r="D26" s="6"/>
       <c r="E26" s="6"/>
       <c r="F26" s="6"/>
       <c r="G26" s="6"/>
       <c r="H26" s="6"/>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I26" s="6"/>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>41813</v>
       </c>
-      <c r="C27">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B27" s="9" t="str">
+        <f>HLOOKUP(WEEKDAY(A27),Sheet1!$A$1:$G$2,2,FALSE)</f>
+        <v>MON</v>
+      </c>
+      <c r="D27">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>41814</v>
       </c>
-      <c r="C28">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B28" s="9" t="str">
+        <f>HLOOKUP(WEEKDAY(A28),Sheet1!$A$1:$G$2,2,FALSE)</f>
+        <v>TUE</v>
+      </c>
+      <c r="D28">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>41815</v>
       </c>
-      <c r="C29">
+      <c r="B29" s="9" t="str">
+        <f>HLOOKUP(WEEKDAY(A29),Sheet1!$A$1:$G$2,2,FALSE)</f>
+        <v>WED</v>
+      </c>
+      <c r="D29">
         <v>3</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>41816</v>
       </c>
-      <c r="C30">
+      <c r="B30" s="9" t="str">
+        <f>HLOOKUP(WEEKDAY(A30),Sheet1!$A$1:$G$2,2,FALSE)</f>
+        <v>THU</v>
+      </c>
+      <c r="D30">
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>41817</v>
       </c>
-      <c r="C31">
+      <c r="B31" s="9" t="str">
+        <f>HLOOKUP(WEEKDAY(A31),Sheet1!$A$1:$G$2,2,FALSE)</f>
+        <v>FRI</v>
+      </c>
+      <c r="D31">
         <v>3</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
         <v>41818</v>
       </c>
-      <c r="B32" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C32" s="3">
+      <c r="B32" s="9" t="str">
+        <f>HLOOKUP(WEEKDAY(A32),Sheet1!$A$1:$G$2,2,FALSE)</f>
+        <v>SAT</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D32" s="3">
         <v>8</v>
       </c>
-      <c r="D32" s="3"/>
       <c r="E32" s="3"/>
       <c r="F32" s="3"/>
       <c r="G32" s="3"/>
       <c r="H32" s="3"/>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I32" s="3"/>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
         <v>41819</v>
       </c>
-      <c r="B33" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C33" s="3">
+      <c r="B33" s="9" t="str">
+        <f>HLOOKUP(WEEKDAY(A33),Sheet1!$A$1:$G$2,2,FALSE)</f>
+        <v>SUN</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D33" s="3">
         <v>8</v>
       </c>
-      <c r="D33" s="3"/>
       <c r="E33" s="3"/>
       <c r="F33" s="3"/>
       <c r="G33" s="3"/>
       <c r="H33" s="3"/>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I33" s="3"/>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>41820</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B34" s="9" t="str">
+        <f>HLOOKUP(WEEKDAY(A34),Sheet1!$A$1:$G$2,2,FALSE)</f>
+        <v>MON</v>
+      </c>
+      <c r="C34" t="s">
         <v>16</v>
       </c>
-      <c r="C34">
+      <c r="D34">
         <v>4</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>41821</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B35" s="9" t="str">
+        <f>HLOOKUP(WEEKDAY(A35),Sheet1!$A$1:$G$2,2,FALSE)</f>
+        <v>TUE</v>
+      </c>
+      <c r="C35" t="s">
         <v>16</v>
       </c>
-      <c r="C35">
+      <c r="D35">
         <v>4</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>41822</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B36" s="9" t="str">
+        <f>HLOOKUP(WEEKDAY(A36),Sheet1!$A$1:$G$2,2,FALSE)</f>
+        <v>WED</v>
+      </c>
+      <c r="C36" t="s">
         <v>16</v>
       </c>
-      <c r="C36">
+      <c r="D36">
         <v>4</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>41823</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B37" s="9" t="str">
+        <f>HLOOKUP(WEEKDAY(A37),Sheet1!$A$1:$G$2,2,FALSE)</f>
+        <v>THU</v>
+      </c>
+      <c r="C37" t="s">
         <v>16</v>
       </c>
-      <c r="C37">
+      <c r="D37">
         <v>5</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>41824</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B38" s="9" t="str">
+        <f>HLOOKUP(WEEKDAY(A38),Sheet1!$A$1:$G$2,2,FALSE)</f>
+        <v>FRI</v>
+      </c>
+      <c r="C38" t="s">
         <v>16</v>
       </c>
-      <c r="C38">
+      <c r="D38">
         <v>6</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="5">
         <v>41825</v>
       </c>
-      <c r="B39" s="6" t="s">
+      <c r="B39" s="9" t="str">
+        <f>HLOOKUP(WEEKDAY(A39),Sheet1!$A$1:$G$2,2,FALSE)</f>
+        <v>SAT</v>
+      </c>
+      <c r="C39" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C39" s="6">
-        <v>2</v>
-      </c>
-      <c r="D39" s="6"/>
+      <c r="D39" s="6">
+        <v>2</v>
+      </c>
       <c r="E39" s="6"/>
       <c r="F39" s="6"/>
       <c r="G39" s="6"/>
       <c r="H39" s="6"/>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I39" s="6"/>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="5">
         <v>41826</v>
       </c>
-      <c r="B40" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="C40" s="6">
+      <c r="B40" s="9" t="str">
+        <f>HLOOKUP(WEEKDAY(A40),Sheet1!$A$1:$G$2,2,FALSE)</f>
+        <v>SUN</v>
+      </c>
+      <c r="C40" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D40" s="6">
         <v>4</v>
       </c>
-      <c r="D40" s="6"/>
       <c r="E40" s="6"/>
       <c r="F40" s="6"/>
       <c r="G40" s="6"/>
       <c r="H40" s="6"/>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I40" s="6"/>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>41827</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B41" s="9" t="str">
+        <f>HLOOKUP(WEEKDAY(A41),Sheet1!$A$1:$G$2,2,FALSE)</f>
+        <v>MON</v>
+      </c>
+      <c r="C41" t="s">
         <v>16</v>
       </c>
-      <c r="C41" s="4">
+      <c r="D41" s="4">
         <v>4</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>41828</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B42" s="9" t="str">
+        <f>HLOOKUP(WEEKDAY(A42),Sheet1!$A$1:$G$2,2,FALSE)</f>
+        <v>TUE</v>
+      </c>
+      <c r="C42" t="s">
         <v>16</v>
       </c>
-      <c r="C42">
+      <c r="D42">
         <v>4</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>41829</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B43" s="9" t="str">
+        <f>HLOOKUP(WEEKDAY(A43),Sheet1!$A$1:$G$2,2,FALSE)</f>
+        <v>WED</v>
+      </c>
+      <c r="C43" t="s">
         <v>16</v>
       </c>
-      <c r="C43">
+      <c r="D43">
         <v>3</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>41830</v>
       </c>
-      <c r="B44" t="s">
-        <v>17</v>
-      </c>
-      <c r="C44">
+      <c r="B44" s="9" t="str">
+        <f>HLOOKUP(WEEKDAY(A44),Sheet1!$A$1:$G$2,2,FALSE)</f>
+        <v>THU</v>
+      </c>
+      <c r="C44" t="s">
+        <v>17</v>
+      </c>
+      <c r="D44">
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>41831</v>
       </c>
-      <c r="C45">
+      <c r="B45" s="9" t="str">
+        <f>HLOOKUP(WEEKDAY(A45),Sheet1!$A$1:$G$2,2,FALSE)</f>
+        <v>FRI</v>
+      </c>
+      <c r="D45">
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="5">
         <v>41832</v>
       </c>
-      <c r="B46" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="C46" s="6">
-        <v>2</v>
-      </c>
-      <c r="D46" s="6"/>
+      <c r="B46" s="9" t="str">
+        <f>HLOOKUP(WEEKDAY(A46),Sheet1!$A$1:$G$2,2,FALSE)</f>
+        <v>SAT</v>
+      </c>
+      <c r="C46" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D46" s="6">
+        <v>2</v>
+      </c>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
       <c r="H46" s="6"/>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I46" s="6"/>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="5">
         <v>41833</v>
       </c>
-      <c r="B47" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="C47" s="6">
+      <c r="B47" s="9" t="str">
+        <f>HLOOKUP(WEEKDAY(A47),Sheet1!$A$1:$G$2,2,FALSE)</f>
+        <v>SUN</v>
+      </c>
+      <c r="C47" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D47" s="6">
         <v>3</v>
       </c>
-      <c r="D47" s="6"/>
       <c r="E47" s="6"/>
       <c r="F47" s="6"/>
       <c r="G47" s="6"/>
       <c r="H47" s="6"/>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I47" s="6"/>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>41834</v>
       </c>
-      <c r="B48" t="s">
-        <v>17</v>
-      </c>
-      <c r="C48">
+      <c r="B48" s="9" t="str">
+        <f>HLOOKUP(WEEKDAY(A48),Sheet1!$A$1:$G$2,2,FALSE)</f>
+        <v>MON</v>
+      </c>
+      <c r="C48" t="s">
+        <v>17</v>
+      </c>
+      <c r="D48">
         <v>5</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>41835</v>
       </c>
-      <c r="B49" t="s">
-        <v>17</v>
-      </c>
-      <c r="C49">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B49" s="9" t="str">
+        <f>HLOOKUP(WEEKDAY(A49),Sheet1!$A$1:$G$2,2,FALSE)</f>
+        <v>TUE</v>
+      </c>
+      <c r="C49" t="s">
+        <v>17</v>
+      </c>
+      <c r="D49">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>41836</v>
       </c>
-      <c r="B50" t="s">
-        <v>17</v>
-      </c>
-      <c r="C50">
+      <c r="B50" s="9" t="str">
+        <f>HLOOKUP(WEEKDAY(A50),Sheet1!$A$1:$G$2,2,FALSE)</f>
+        <v>WED</v>
+      </c>
+      <c r="C50" t="s">
+        <v>17</v>
+      </c>
+      <c r="D50">
         <v>4</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>41837</v>
       </c>
-      <c r="B51" t="s">
-        <v>17</v>
-      </c>
-      <c r="C51">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B51" s="9" t="str">
+        <f>HLOOKUP(WEEKDAY(A51),Sheet1!$A$1:$G$2,2,FALSE)</f>
+        <v>THU</v>
+      </c>
+      <c r="C51" t="s">
+        <v>17</v>
+      </c>
+      <c r="D51">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>41838</v>
       </c>
-      <c r="B52" t="s">
-        <v>17</v>
-      </c>
-      <c r="C52">
+      <c r="B52" s="9" t="str">
+        <f>HLOOKUP(WEEKDAY(A52),Sheet1!$A$1:$G$2,2,FALSE)</f>
+        <v>FRI</v>
+      </c>
+      <c r="C52" t="s">
+        <v>17</v>
+      </c>
+      <c r="D52">
         <v>4</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>41839</v>
       </c>
-      <c r="B53" t="s">
-        <v>17</v>
-      </c>
-      <c r="C53">
+      <c r="B53" s="9" t="str">
+        <f>HLOOKUP(WEEKDAY(A53),Sheet1!$A$1:$G$2,2,FALSE)</f>
+        <v>SAT</v>
+      </c>
+      <c r="C53" t="s">
+        <v>17</v>
+      </c>
+      <c r="D53">
         <v>4</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>41841</v>
       </c>
-      <c r="B54" t="s">
-        <v>17</v>
-      </c>
-      <c r="C54">
+      <c r="B54" s="9" t="str">
+        <f>HLOOKUP(WEEKDAY(A54),Sheet1!$A$1:$G$2,2,FALSE)</f>
+        <v>MON</v>
+      </c>
+      <c r="C54" t="s">
+        <v>17</v>
+      </c>
+      <c r="D54">
         <v>4</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>41842</v>
       </c>
-      <c r="B55" t="s">
-        <v>17</v>
-      </c>
-      <c r="C55">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B55" s="9" t="str">
+        <f>HLOOKUP(WEEKDAY(A55),Sheet1!$A$1:$G$2,2,FALSE)</f>
+        <v>TUE</v>
+      </c>
+      <c r="C55" t="s">
+        <v>17</v>
+      </c>
+      <c r="D55">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>41843</v>
       </c>
-      <c r="B56" t="s">
-        <v>17</v>
-      </c>
-      <c r="C56">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B56" s="9" t="str">
+        <f>HLOOKUP(WEEKDAY(A56),Sheet1!$A$1:$G$2,2,FALSE)</f>
+        <v>WED</v>
+      </c>
+      <c r="C56" t="s">
+        <v>17</v>
+      </c>
+      <c r="D56">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>41844</v>
       </c>
-      <c r="B57" t="s">
-        <v>17</v>
-      </c>
-      <c r="C57">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B57" s="9" t="str">
+        <f>HLOOKUP(WEEKDAY(A57),Sheet1!$A$1:$G$2,2,FALSE)</f>
+        <v>THU</v>
+      </c>
+      <c r="C57" t="s">
+        <v>17</v>
+      </c>
+      <c r="D57">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>41845</v>
       </c>
-      <c r="B58" t="s">
-        <v>17</v>
-      </c>
-      <c r="C58">
+      <c r="B58" s="9" t="str">
+        <f>HLOOKUP(WEEKDAY(A58),Sheet1!$A$1:$G$2,2,FALSE)</f>
+        <v>FRI</v>
+      </c>
+      <c r="C58" t="s">
+        <v>17</v>
+      </c>
+      <c r="D58">
         <v>5</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <v>41846</v>
       </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B59" s="9" t="str">
+        <f>HLOOKUP(WEEKDAY(A59),Sheet1!$A$1:$G$2,2,FALSE)</f>
+        <v>SAT</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <v>41847</v>
       </c>
-      <c r="B60" t="s">
+      <c r="B60" s="9" t="str">
+        <f>HLOOKUP(WEEKDAY(A60),Sheet1!$A$1:$G$2,2,FALSE)</f>
+        <v>SUN</v>
+      </c>
+      <c r="C60" t="s">
         <v>16</v>
       </c>
-      <c r="C60">
+      <c r="D60">
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <v>41848</v>
       </c>
-      <c r="B61" t="s">
-        <v>17</v>
-      </c>
-      <c r="C61">
+      <c r="B61" s="9" t="str">
+        <f>HLOOKUP(WEEKDAY(A61),Sheet1!$A$1:$G$2,2,FALSE)</f>
+        <v>MON</v>
+      </c>
+      <c r="C61" t="s">
+        <v>17</v>
+      </c>
+      <c r="D61">
         <v>3</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
         <v>41849</v>
       </c>
-      <c r="B62" t="s">
-        <v>17</v>
-      </c>
-      <c r="C62">
+      <c r="B62" s="9" t="str">
+        <f>HLOOKUP(WEEKDAY(A62),Sheet1!$A$1:$G$2,2,FALSE)</f>
+        <v>TUE</v>
+      </c>
+      <c r="C62" t="s">
+        <v>17</v>
+      </c>
+      <c r="D62">
         <v>3</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <v>41850</v>
       </c>
-      <c r="B63" t="s">
-        <v>17</v>
-      </c>
-      <c r="C63">
+      <c r="B63" s="9" t="str">
+        <f>HLOOKUP(WEEKDAY(A63),Sheet1!$A$1:$G$2,2,FALSE)</f>
+        <v>WED</v>
+      </c>
+      <c r="C63" t="s">
+        <v>17</v>
+      </c>
+      <c r="D63">
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <v>41851</v>
       </c>
-      <c r="B64" t="s">
-        <v>17</v>
-      </c>
-      <c r="C64">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B64" s="9" t="str">
+        <f>HLOOKUP(WEEKDAY(A64),Sheet1!$A$1:$G$2,2,FALSE)</f>
+        <v>THU</v>
+      </c>
+      <c r="C64" t="s">
+        <v>17</v>
+      </c>
+      <c r="D64">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <v>41852</v>
       </c>
-      <c r="B65" t="s">
-        <v>17</v>
-      </c>
-      <c r="C65">
+      <c r="B65" s="9" t="str">
+        <f>HLOOKUP(WEEKDAY(A65),Sheet1!$A$1:$G$2,2,FALSE)</f>
+        <v>FRI</v>
+      </c>
+      <c r="C65" t="s">
+        <v>17</v>
+      </c>
+      <c r="D65">
         <v>3</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <v>41853</v>
       </c>
-      <c r="B66" t="s">
-        <v>17</v>
-      </c>
-      <c r="C66">
+      <c r="B66" s="9" t="str">
+        <f>HLOOKUP(WEEKDAY(A66),Sheet1!$A$1:$G$2,2,FALSE)</f>
+        <v>SAT</v>
+      </c>
+      <c r="C66" t="s">
+        <v>17</v>
+      </c>
+      <c r="D66">
         <v>5</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <v>41854</v>
       </c>
-      <c r="B67" t="s">
-        <v>17</v>
-      </c>
-      <c r="C67">
+      <c r="B67" s="9" t="str">
+        <f>HLOOKUP(WEEKDAY(A67),Sheet1!$A$1:$G$2,2,FALSE)</f>
+        <v>SUN</v>
+      </c>
+      <c r="C67" t="s">
+        <v>17</v>
+      </c>
+      <c r="D67">
         <v>6</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <v>41855</v>
       </c>
-      <c r="B68" t="s">
-        <v>17</v>
-      </c>
-      <c r="C68">
+      <c r="B68" s="9" t="str">
+        <f>HLOOKUP(WEEKDAY(A68),Sheet1!$A$1:$G$2,2,FALSE)</f>
+        <v>MON</v>
+      </c>
+      <c r="C68" t="s">
+        <v>17</v>
+      </c>
+      <c r="D68">
         <v>8</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
         <v>41856</v>
       </c>
-      <c r="B69" t="s">
+      <c r="B69" s="9" t="str">
+        <f>HLOOKUP(WEEKDAY(A69),Sheet1!$A$1:$G$2,2,FALSE)</f>
+        <v>TUE</v>
+      </c>
+      <c r="C69" t="s">
         <v>16</v>
       </c>
-      <c r="C69">
+      <c r="D69">
         <v>6</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
         <v>41857</v>
       </c>
-      <c r="B70" t="s">
+      <c r="B70" s="9" t="str">
+        <f>HLOOKUP(WEEKDAY(A70),Sheet1!$A$1:$G$2,2,FALSE)</f>
+        <v>WED</v>
+      </c>
+      <c r="C70" t="s">
         <v>16</v>
       </c>
-      <c r="C70">
+      <c r="D70">
         <v>8</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
         <v>41858</v>
       </c>
-      <c r="B71" t="s">
-        <v>17</v>
-      </c>
-      <c r="C71">
+      <c r="B71" s="9" t="str">
+        <f>HLOOKUP(WEEKDAY(A71),Sheet1!$A$1:$G$2,2,FALSE)</f>
+        <v>THU</v>
+      </c>
+      <c r="C71" t="s">
+        <v>17</v>
+      </c>
+      <c r="D71">
         <v>4</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
         <v>41859</v>
       </c>
-      <c r="B72" t="s">
-        <v>17</v>
-      </c>
-      <c r="C72">
+      <c r="B72" s="9" t="str">
+        <f>HLOOKUP(WEEKDAY(A72),Sheet1!$A$1:$G$2,2,FALSE)</f>
+        <v>FRI</v>
+      </c>
+      <c r="C72" t="s">
+        <v>17</v>
+      </c>
+      <c r="D72">
         <v>8</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A73" s="1">
+        <v>41860</v>
+      </c>
+      <c r="B73" s="9" t="str">
+        <f>HLOOKUP(WEEKDAY(A73),Sheet1!$A$1:$G$2,2,FALSE)</f>
+        <v>SAT</v>
+      </c>
+      <c r="D73">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A74" s="1">
+        <v>41861</v>
+      </c>
+      <c r="B74" s="9" t="str">
+        <f>HLOOKUP(WEEKDAY(A74),Sheet1!$A$1:$G$2,2,FALSE)</f>
+        <v>SUN</v>
+      </c>
+      <c r="D74">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A75" s="1">
+        <v>41862</v>
+      </c>
+      <c r="B75" s="9" t="str">
+        <f>HLOOKUP(WEEKDAY(A75),Sheet1!$A$1:$G$2,2,FALSE)</f>
+        <v>MON</v>
+      </c>
+      <c r="D75">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A76" s="1">
+        <v>41863</v>
+      </c>
+      <c r="B76" s="9" t="str">
+        <f>HLOOKUP(WEEKDAY(A76),Sheet1!$A$1:$G$2,2,FALSE)</f>
+        <v>TUE</v>
+      </c>
+      <c r="D76">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A77" s="1">
+        <v>41864</v>
+      </c>
+      <c r="B77" s="9" t="str">
+        <f>HLOOKUP(WEEKDAY(A77),Sheet1!$A$1:$G$2,2,FALSE)</f>
+        <v>WED</v>
+      </c>
+      <c r="D77">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A78" s="1">
+        <v>41865</v>
+      </c>
+      <c r="B78" s="9" t="str">
+        <f>HLOOKUP(WEEKDAY(A78),Sheet1!$A$1:$G$2,2,FALSE)</f>
+        <v>THU</v>
+      </c>
+      <c r="D78">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A79" s="1">
+        <v>41866</v>
+      </c>
+      <c r="B79" s="9" t="str">
+        <f>HLOOKUP(WEEKDAY(A79),Sheet1!$A$1:$G$2,2,FALSE)</f>
+        <v>FRI</v>
+      </c>
+      <c r="D79">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A80" s="1">
+        <v>41867</v>
+      </c>
+      <c r="B80" s="9" t="str">
+        <f>HLOOKUP(WEEKDAY(A80),Sheet1!$A$1:$G$2,2,FALSE)</f>
+        <v>SAT</v>
+      </c>
+      <c r="D80">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A81" s="1">
+        <v>41868</v>
+      </c>
+      <c r="B81" s="9" t="str">
+        <f>HLOOKUP(WEEKDAY(A81),Sheet1!$A$1:$G$2,2,FALSE)</f>
+        <v>SUN</v>
+      </c>
+      <c r="D81">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A82" s="1">
+        <v>41869</v>
+      </c>
+      <c r="B82" s="9" t="str">
+        <f>HLOOKUP(WEEKDAY(A82),Sheet1!$A$1:$G$2,2,FALSE)</f>
+        <v>MON</v>
+      </c>
+      <c r="D82">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A83" s="1">
+        <v>41870</v>
+      </c>
+      <c r="B83" s="9" t="str">
+        <f>HLOOKUP(WEEKDAY(A83),Sheet1!$A$1:$G$2,2,FALSE)</f>
+        <v>TUE</v>
+      </c>
+      <c r="D83">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A84" s="1">
+        <v>41871</v>
+      </c>
+      <c r="B84" s="9" t="str">
+        <f>HLOOKUP(WEEKDAY(A84),Sheet1!$A$1:$G$2,2,FALSE)</f>
+        <v>WED</v>
+      </c>
+      <c r="D84">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A85" s="1">
+        <v>41872</v>
+      </c>
+      <c r="B85" s="9" t="str">
+        <f>HLOOKUP(WEEKDAY(A85),Sheet1!$A$1:$G$2,2,FALSE)</f>
+        <v>THU</v>
+      </c>
+      <c r="D85">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A86" s="1">
+        <v>41873</v>
+      </c>
+      <c r="B86" s="9" t="str">
+        <f>HLOOKUP(WEEKDAY(A86),Sheet1!$A$1:$G$2,2,FALSE)</f>
+        <v>FRI</v>
+      </c>
+      <c r="D86">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A87" s="1">
+        <v>41874</v>
+      </c>
+      <c r="B87" s="9" t="str">
+        <f>HLOOKUP(WEEKDAY(A87),Sheet1!$A$1:$G$2,2,FALSE)</f>
+        <v>SAT</v>
+      </c>
+      <c r="D87">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A88" s="1">
+        <v>41875</v>
+      </c>
+      <c r="B88" s="9" t="str">
+        <f>HLOOKUP(WEEKDAY(A88),Sheet1!$A$1:$G$2,2,FALSE)</f>
+        <v>SUN</v>
+      </c>
+      <c r="D88">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A89" s="1">
+        <v>41876</v>
+      </c>
+      <c r="B89" s="9" t="str">
+        <f>HLOOKUP(WEEKDAY(A89),Sheet1!$A$1:$G$2,2,FALSE)</f>
+        <v>MON</v>
+      </c>
+      <c r="D89">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A90" s="1">
+        <v>41877</v>
+      </c>
+      <c r="B90" s="9" t="str">
+        <f>HLOOKUP(WEEKDAY(A90),Sheet1!$A$1:$G$2,2,FALSE)</f>
+        <v>TUE</v>
+      </c>
+      <c r="D90">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A91" s="1">
+        <v>41878</v>
+      </c>
+      <c r="B91" s="9" t="str">
+        <f>HLOOKUP(WEEKDAY(A91),Sheet1!$A$1:$G$2,2,FALSE)</f>
+        <v>WED</v>
+      </c>
+      <c r="D91">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A92" s="1">
+        <v>41879</v>
+      </c>
+      <c r="B92" s="9" t="str">
+        <f>HLOOKUP(WEEKDAY(A92),Sheet1!$A$1:$G$2,2,FALSE)</f>
+        <v>THU</v>
+      </c>
+      <c r="D92">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A93" s="1">
+        <v>41880</v>
+      </c>
+      <c r="B93" s="9" t="str">
+        <f>HLOOKUP(WEEKDAY(A93),Sheet1!$A$1:$G$2,2,FALSE)</f>
+        <v>FRI</v>
+      </c>
+      <c r="D93">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A94" s="1">
+        <v>41881</v>
+      </c>
+      <c r="B94" s="9" t="str">
+        <f>HLOOKUP(WEEKDAY(A94),Sheet1!$A$1:$G$2,2,FALSE)</f>
+        <v>SAT</v>
+      </c>
+      <c r="D94">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A95" s="1">
+        <v>41882</v>
+      </c>
+      <c r="B95" s="9" t="str">
+        <f>HLOOKUP(WEEKDAY(A95),Sheet1!$A$1:$G$2,2,FALSE)</f>
+        <v>SUN</v>
+      </c>
+      <c r="D95">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A96" s="1">
+        <v>41883</v>
+      </c>
+      <c r="B96" s="9" t="str">
+        <f>HLOOKUP(WEEKDAY(A96),Sheet1!$A$1:$G$2,2,FALSE)</f>
+        <v>MON</v>
+      </c>
+      <c r="D96">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A97" s="1">
+        <v>41884</v>
+      </c>
+      <c r="B97" s="9" t="str">
+        <f>HLOOKUP(WEEKDAY(A97),Sheet1!$A$1:$G$2,2,FALSE)</f>
+        <v>TUE</v>
+      </c>
+      <c r="D97">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A98" s="1">
+        <v>41885</v>
+      </c>
+      <c r="B98" s="9" t="str">
+        <f>HLOOKUP(WEEKDAY(A98),Sheet1!$A$1:$G$2,2,FALSE)</f>
+        <v>WED</v>
+      </c>
+      <c r="D98">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A99" s="1">
+        <v>41886</v>
+      </c>
+      <c r="B99" s="9" t="str">
+        <f>HLOOKUP(WEEKDAY(A99),Sheet1!$A$1:$G$2,2,FALSE)</f>
+        <v>THU</v>
+      </c>
+      <c r="D99">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A100" s="1">
+        <v>41887</v>
+      </c>
+      <c r="B100" s="9" t="str">
+        <f>HLOOKUP(WEEKDAY(A100),Sheet1!$A$1:$G$2,2,FALSE)</f>
+        <v>FRI</v>
+      </c>
+      <c r="D100">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A101" s="1">
+        <v>41888</v>
+      </c>
+      <c r="B101" s="9" t="str">
+        <f>HLOOKUP(WEEKDAY(A101),Sheet1!$A$1:$G$2,2,FALSE)</f>
+        <v>SAT</v>
+      </c>
+      <c r="D101">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A102" s="1">
+        <v>41889</v>
+      </c>
+      <c r="B102" s="9" t="str">
+        <f>HLOOKUP(WEEKDAY(A102),Sheet1!$A$1:$G$2,2,FALSE)</f>
+        <v>SUN</v>
+      </c>
+      <c r="D102">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A103" s="1">
+        <v>41890</v>
+      </c>
+      <c r="B103" s="9" t="str">
+        <f>HLOOKUP(WEEKDAY(A103),Sheet1!$A$1:$G$2,2,FALSE)</f>
+        <v>MON</v>
+      </c>
+      <c r="D103">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A104" s="1">
+        <v>41891</v>
+      </c>
+      <c r="B104" s="9" t="str">
+        <f>HLOOKUP(WEEKDAY(A104),Sheet1!$A$1:$G$2,2,FALSE)</f>
+        <v>TUE</v>
+      </c>
+      <c r="D104">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A105" s="1">
+        <v>41892</v>
+      </c>
+      <c r="B105" s="9" t="str">
+        <f>HLOOKUP(WEEKDAY(A105),Sheet1!$A$1:$G$2,2,FALSE)</f>
+        <v>WED</v>
+      </c>
+      <c r="D105">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A106" s="1">
+        <v>41893</v>
+      </c>
+      <c r="B106" s="9" t="str">
+        <f>HLOOKUP(WEEKDAY(A106),Sheet1!$A$1:$G$2,2,FALSE)</f>
+        <v>THU</v>
+      </c>
+      <c r="D106">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A107" s="1">
+        <v>41894</v>
+      </c>
+      <c r="B107" s="9" t="str">
+        <f>HLOOKUP(WEEKDAY(A107),Sheet1!$A$1:$G$2,2,FALSE)</f>
+        <v>FRI</v>
+      </c>
+      <c r="D107">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A108" s="1">
+        <v>41895</v>
+      </c>
+      <c r="B108" s="9" t="str">
+        <f>HLOOKUP(WEEKDAY(A108),Sheet1!$A$1:$G$2,2,FALSE)</f>
+        <v>SAT</v>
+      </c>
+      <c r="D108">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A109" s="1">
+        <v>41896</v>
+      </c>
+      <c r="B109" s="9" t="str">
+        <f>HLOOKUP(WEEKDAY(A109),Sheet1!$A$1:$G$2,2,FALSE)</f>
+        <v>SUN</v>
+      </c>
+      <c r="D109">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A110" s="1">
+        <v>41897</v>
+      </c>
+      <c r="B110" s="9" t="str">
+        <f>HLOOKUP(WEEKDAY(A110),Sheet1!$A$1:$G$2,2,FALSE)</f>
+        <v>MON</v>
+      </c>
+      <c r="D110">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A111" s="1">
+        <v>41898</v>
+      </c>
+      <c r="B111" s="9" t="str">
+        <f>HLOOKUP(WEEKDAY(A111),Sheet1!$A$1:$G$2,2,FALSE)</f>
+        <v>TUE</v>
+      </c>
+      <c r="D111">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A112" s="1">
+        <v>41899</v>
+      </c>
+      <c r="B112" s="9" t="str">
+        <f>HLOOKUP(WEEKDAY(A112),Sheet1!$A$1:$G$2,2,FALSE)</f>
+        <v>WED</v>
+      </c>
+      <c r="D112">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -1574,4 +2357,65 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <v>1</v>
+      </c>
+      <c r="B1">
+        <v>2</v>
+      </c>
+      <c r="C1">
+        <v>3</v>
+      </c>
+      <c r="D1">
+        <v>4</v>
+      </c>
+      <c r="E1">
+        <v>5</v>
+      </c>
+      <c r="F1">
+        <v>6</v>
+      </c>
+      <c r="G1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2" t="s">
+        <v>44</v>
+      </c>
+      <c r="F2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
improve oneUnknow to fix intervals
</commit_message>
<xml_diff>
--- a/Test.xlsx
+++ b/Test.xlsx
@@ -4,20 +4,21 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="19440" windowHeight="7935" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="19440" windowHeight="7935" activeTab="4"/>
   </bookViews>
   <sheets>
-    <sheet name="Testcases" sheetId="1" r:id="rId1"/>
-    <sheet name="Time" sheetId="2" r:id="rId2"/>
-    <sheet name="Tasks" sheetId="3" r:id="rId3"/>
-    <sheet name="Sheet1" sheetId="4" r:id="rId4"/>
+    <sheet name="Constants" sheetId="4" r:id="rId1"/>
+    <sheet name="Testcases" sheetId="1" r:id="rId2"/>
+    <sheet name="Time" sheetId="2" r:id="rId3"/>
+    <sheet name="Tasks" sheetId="3" r:id="rId4"/>
+    <sheet name="Log" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="48">
   <si>
     <t>f(x,y)=x+y</t>
   </si>
@@ -158,13 +159,16 @@
   </si>
   <si>
     <t>SAT</t>
+  </si>
+  <si>
+    <t>Add color to ImageData</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -176,6 +180,20 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF555555"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -210,10 +228,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="15" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
@@ -224,8 +243,12 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="1" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -525,6 +548,67 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H25" sqref="H25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <v>1</v>
+      </c>
+      <c r="B1">
+        <v>2</v>
+      </c>
+      <c r="C1">
+        <v>3</v>
+      </c>
+      <c r="D1">
+        <v>4</v>
+      </c>
+      <c r="E1">
+        <v>5</v>
+      </c>
+      <c r="F1">
+        <v>6</v>
+      </c>
+      <c r="G1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2" t="s">
+        <v>44</v>
+      </c>
+      <c r="F2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -664,12 +748,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I112"/>
+  <dimension ref="A1:I154"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="D113" sqref="D113"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -740,7 +824,7 @@
         <v>41790</v>
       </c>
       <c r="B4" s="9" t="str">
-        <f>HLOOKUP(WEEKDAY(A4),Sheet1!$A$1:$G$2,2,FALSE)</f>
+        <f>HLOOKUP(WEEKDAY(A4),Constants!$A$1:$G$2,2,FALSE)</f>
         <v>SAT</v>
       </c>
       <c r="C4" s="6"/>
@@ -758,7 +842,7 @@
         <v>41791</v>
       </c>
       <c r="B5" s="9" t="str">
-        <f>HLOOKUP(WEEKDAY(A5),Sheet1!$A$1:$G$2,2,FALSE)</f>
+        <f>HLOOKUP(WEEKDAY(A5),Constants!$A$1:$G$2,2,FALSE)</f>
         <v>SUN</v>
       </c>
       <c r="C5" s="6"/>
@@ -776,7 +860,7 @@
         <v>41792</v>
       </c>
       <c r="B6" s="9" t="str">
-        <f>HLOOKUP(WEEKDAY(A6),Sheet1!$A$1:$G$2,2,FALSE)</f>
+        <f>HLOOKUP(WEEKDAY(A6),Constants!$A$1:$G$2,2,FALSE)</f>
         <v>MON</v>
       </c>
       <c r="D6">
@@ -788,7 +872,7 @@
         <v>41793</v>
       </c>
       <c r="B7" s="9" t="str">
-        <f>HLOOKUP(WEEKDAY(A7),Sheet1!$A$1:$G$2,2,FALSE)</f>
+        <f>HLOOKUP(WEEKDAY(A7),Constants!$A$1:$G$2,2,FALSE)</f>
         <v>TUE</v>
       </c>
       <c r="D7">
@@ -800,7 +884,7 @@
         <v>41794</v>
       </c>
       <c r="B8" s="9" t="str">
-        <f>HLOOKUP(WEEKDAY(A8),Sheet1!$A$1:$G$2,2,FALSE)</f>
+        <f>HLOOKUP(WEEKDAY(A8),Constants!$A$1:$G$2,2,FALSE)</f>
         <v>WED</v>
       </c>
       <c r="D8">
@@ -812,7 +896,7 @@
         <v>41795</v>
       </c>
       <c r="B9" s="9" t="str">
-        <f>HLOOKUP(WEEKDAY(A9),Sheet1!$A$1:$G$2,2,FALSE)</f>
+        <f>HLOOKUP(WEEKDAY(A9),Constants!$A$1:$G$2,2,FALSE)</f>
         <v>THU</v>
       </c>
       <c r="D9">
@@ -824,7 +908,7 @@
         <v>41796</v>
       </c>
       <c r="B10" s="9" t="str">
-        <f>HLOOKUP(WEEKDAY(A10),Sheet1!$A$1:$G$2,2,FALSE)</f>
+        <f>HLOOKUP(WEEKDAY(A10),Constants!$A$1:$G$2,2,FALSE)</f>
         <v>FRI</v>
       </c>
       <c r="D10">
@@ -836,7 +920,7 @@
         <v>41797</v>
       </c>
       <c r="B11" s="9" t="str">
-        <f>HLOOKUP(WEEKDAY(A11),Sheet1!$A$1:$G$2,2,FALSE)</f>
+        <f>HLOOKUP(WEEKDAY(A11),Constants!$A$1:$G$2,2,FALSE)</f>
         <v>SAT</v>
       </c>
       <c r="C11" s="6"/>
@@ -854,7 +938,7 @@
         <v>41798</v>
       </c>
       <c r="B12" s="9" t="str">
-        <f>HLOOKUP(WEEKDAY(A12),Sheet1!$A$1:$G$2,2,FALSE)</f>
+        <f>HLOOKUP(WEEKDAY(A12),Constants!$A$1:$G$2,2,FALSE)</f>
         <v>SUN</v>
       </c>
       <c r="C12" s="6"/>
@@ -872,7 +956,7 @@
         <v>41799</v>
       </c>
       <c r="B13" s="9" t="str">
-        <f>HLOOKUP(WEEKDAY(A13),Sheet1!$A$1:$G$2,2,FALSE)</f>
+        <f>HLOOKUP(WEEKDAY(A13),Constants!$A$1:$G$2,2,FALSE)</f>
         <v>MON</v>
       </c>
       <c r="D13">
@@ -884,7 +968,7 @@
         <v>41800</v>
       </c>
       <c r="B14" s="9" t="str">
-        <f>HLOOKUP(WEEKDAY(A14),Sheet1!$A$1:$G$2,2,FALSE)</f>
+        <f>HLOOKUP(WEEKDAY(A14),Constants!$A$1:$G$2,2,FALSE)</f>
         <v>TUE</v>
       </c>
       <c r="D14">
@@ -896,7 +980,7 @@
         <v>41801</v>
       </c>
       <c r="B15" s="9" t="str">
-        <f>HLOOKUP(WEEKDAY(A15),Sheet1!$A$1:$G$2,2,FALSE)</f>
+        <f>HLOOKUP(WEEKDAY(A15),Constants!$A$1:$G$2,2,FALSE)</f>
         <v>WED</v>
       </c>
       <c r="D15">
@@ -908,7 +992,7 @@
         <v>41802</v>
       </c>
       <c r="B16" s="9" t="str">
-        <f>HLOOKUP(WEEKDAY(A16),Sheet1!$A$1:$G$2,2,FALSE)</f>
+        <f>HLOOKUP(WEEKDAY(A16),Constants!$A$1:$G$2,2,FALSE)</f>
         <v>THU</v>
       </c>
       <c r="D16">
@@ -920,7 +1004,7 @@
         <v>41803</v>
       </c>
       <c r="B17" s="9" t="str">
-        <f>HLOOKUP(WEEKDAY(A17),Sheet1!$A$1:$G$2,2,FALSE)</f>
+        <f>HLOOKUP(WEEKDAY(A17),Constants!$A$1:$G$2,2,FALSE)</f>
         <v>FRI</v>
       </c>
       <c r="D17">
@@ -932,7 +1016,7 @@
         <v>41804</v>
       </c>
       <c r="B18" s="9" t="str">
-        <f>HLOOKUP(WEEKDAY(A18),Sheet1!$A$1:$G$2,2,FALSE)</f>
+        <f>HLOOKUP(WEEKDAY(A18),Constants!$A$1:$G$2,2,FALSE)</f>
         <v>SAT</v>
       </c>
       <c r="C18" s="6"/>
@@ -950,7 +1034,7 @@
         <v>41805</v>
       </c>
       <c r="B19" s="9" t="str">
-        <f>HLOOKUP(WEEKDAY(A19),Sheet1!$A$1:$G$2,2,FALSE)</f>
+        <f>HLOOKUP(WEEKDAY(A19),Constants!$A$1:$G$2,2,FALSE)</f>
         <v>SUN</v>
       </c>
       <c r="C19" s="6"/>
@@ -968,7 +1052,7 @@
         <v>41806</v>
       </c>
       <c r="B20" s="9" t="str">
-        <f>HLOOKUP(WEEKDAY(A20),Sheet1!$A$1:$G$2,2,FALSE)</f>
+        <f>HLOOKUP(WEEKDAY(A20),Constants!$A$1:$G$2,2,FALSE)</f>
         <v>MON</v>
       </c>
       <c r="D20">
@@ -980,7 +1064,7 @@
         <v>41807</v>
       </c>
       <c r="B21" s="9" t="str">
-        <f>HLOOKUP(WEEKDAY(A21),Sheet1!$A$1:$G$2,2,FALSE)</f>
+        <f>HLOOKUP(WEEKDAY(A21),Constants!$A$1:$G$2,2,FALSE)</f>
         <v>TUE</v>
       </c>
       <c r="D21">
@@ -992,7 +1076,7 @@
         <v>41808</v>
       </c>
       <c r="B22" s="9" t="str">
-        <f>HLOOKUP(WEEKDAY(A22),Sheet1!$A$1:$G$2,2,FALSE)</f>
+        <f>HLOOKUP(WEEKDAY(A22),Constants!$A$1:$G$2,2,FALSE)</f>
         <v>WED</v>
       </c>
       <c r="D22">
@@ -1004,7 +1088,7 @@
         <v>41809</v>
       </c>
       <c r="B23" s="9" t="str">
-        <f>HLOOKUP(WEEKDAY(A23),Sheet1!$A$1:$G$2,2,FALSE)</f>
+        <f>HLOOKUP(WEEKDAY(A23),Constants!$A$1:$G$2,2,FALSE)</f>
         <v>THU</v>
       </c>
       <c r="D23">
@@ -1016,7 +1100,7 @@
         <v>41810</v>
       </c>
       <c r="B24" s="9" t="str">
-        <f>HLOOKUP(WEEKDAY(A24),Sheet1!$A$1:$G$2,2,FALSE)</f>
+        <f>HLOOKUP(WEEKDAY(A24),Constants!$A$1:$G$2,2,FALSE)</f>
         <v>FRI</v>
       </c>
       <c r="D24">
@@ -1028,7 +1112,7 @@
         <v>41811</v>
       </c>
       <c r="B25" s="9" t="str">
-        <f>HLOOKUP(WEEKDAY(A25),Sheet1!$A$1:$G$2,2,FALSE)</f>
+        <f>HLOOKUP(WEEKDAY(A25),Constants!$A$1:$G$2,2,FALSE)</f>
         <v>SAT</v>
       </c>
       <c r="C25" s="6"/>
@@ -1046,7 +1130,7 @@
         <v>41812</v>
       </c>
       <c r="B26" s="9" t="str">
-        <f>HLOOKUP(WEEKDAY(A26),Sheet1!$A$1:$G$2,2,FALSE)</f>
+        <f>HLOOKUP(WEEKDAY(A26),Constants!$A$1:$G$2,2,FALSE)</f>
         <v>SUN</v>
       </c>
       <c r="C26" s="6"/>
@@ -1064,7 +1148,7 @@
         <v>41813</v>
       </c>
       <c r="B27" s="9" t="str">
-        <f>HLOOKUP(WEEKDAY(A27),Sheet1!$A$1:$G$2,2,FALSE)</f>
+        <f>HLOOKUP(WEEKDAY(A27),Constants!$A$1:$G$2,2,FALSE)</f>
         <v>MON</v>
       </c>
       <c r="D27">
@@ -1076,7 +1160,7 @@
         <v>41814</v>
       </c>
       <c r="B28" s="9" t="str">
-        <f>HLOOKUP(WEEKDAY(A28),Sheet1!$A$1:$G$2,2,FALSE)</f>
+        <f>HLOOKUP(WEEKDAY(A28),Constants!$A$1:$G$2,2,FALSE)</f>
         <v>TUE</v>
       </c>
       <c r="D28">
@@ -1088,7 +1172,7 @@
         <v>41815</v>
       </c>
       <c r="B29" s="9" t="str">
-        <f>HLOOKUP(WEEKDAY(A29),Sheet1!$A$1:$G$2,2,FALSE)</f>
+        <f>HLOOKUP(WEEKDAY(A29),Constants!$A$1:$G$2,2,FALSE)</f>
         <v>WED</v>
       </c>
       <c r="D29">
@@ -1100,7 +1184,7 @@
         <v>41816</v>
       </c>
       <c r="B30" s="9" t="str">
-        <f>HLOOKUP(WEEKDAY(A30),Sheet1!$A$1:$G$2,2,FALSE)</f>
+        <f>HLOOKUP(WEEKDAY(A30),Constants!$A$1:$G$2,2,FALSE)</f>
         <v>THU</v>
       </c>
       <c r="D30">
@@ -1112,7 +1196,7 @@
         <v>41817</v>
       </c>
       <c r="B31" s="9" t="str">
-        <f>HLOOKUP(WEEKDAY(A31),Sheet1!$A$1:$G$2,2,FALSE)</f>
+        <f>HLOOKUP(WEEKDAY(A31),Constants!$A$1:$G$2,2,FALSE)</f>
         <v>FRI</v>
       </c>
       <c r="D31">
@@ -1124,7 +1208,7 @@
         <v>41818</v>
       </c>
       <c r="B32" s="9" t="str">
-        <f>HLOOKUP(WEEKDAY(A32),Sheet1!$A$1:$G$2,2,FALSE)</f>
+        <f>HLOOKUP(WEEKDAY(A32),Constants!$A$1:$G$2,2,FALSE)</f>
         <v>SAT</v>
       </c>
       <c r="C32" s="3" t="s">
@@ -1144,7 +1228,7 @@
         <v>41819</v>
       </c>
       <c r="B33" s="9" t="str">
-        <f>HLOOKUP(WEEKDAY(A33),Sheet1!$A$1:$G$2,2,FALSE)</f>
+        <f>HLOOKUP(WEEKDAY(A33),Constants!$A$1:$G$2,2,FALSE)</f>
         <v>SUN</v>
       </c>
       <c r="C33" s="3" t="s">
@@ -1164,7 +1248,7 @@
         <v>41820</v>
       </c>
       <c r="B34" s="9" t="str">
-        <f>HLOOKUP(WEEKDAY(A34),Sheet1!$A$1:$G$2,2,FALSE)</f>
+        <f>HLOOKUP(WEEKDAY(A34),Constants!$A$1:$G$2,2,FALSE)</f>
         <v>MON</v>
       </c>
       <c r="C34" t="s">
@@ -1179,7 +1263,7 @@
         <v>41821</v>
       </c>
       <c r="B35" s="9" t="str">
-        <f>HLOOKUP(WEEKDAY(A35),Sheet1!$A$1:$G$2,2,FALSE)</f>
+        <f>HLOOKUP(WEEKDAY(A35),Constants!$A$1:$G$2,2,FALSE)</f>
         <v>TUE</v>
       </c>
       <c r="C35" t="s">
@@ -1194,7 +1278,7 @@
         <v>41822</v>
       </c>
       <c r="B36" s="9" t="str">
-        <f>HLOOKUP(WEEKDAY(A36),Sheet1!$A$1:$G$2,2,FALSE)</f>
+        <f>HLOOKUP(WEEKDAY(A36),Constants!$A$1:$G$2,2,FALSE)</f>
         <v>WED</v>
       </c>
       <c r="C36" t="s">
@@ -1209,7 +1293,7 @@
         <v>41823</v>
       </c>
       <c r="B37" s="9" t="str">
-        <f>HLOOKUP(WEEKDAY(A37),Sheet1!$A$1:$G$2,2,FALSE)</f>
+        <f>HLOOKUP(WEEKDAY(A37),Constants!$A$1:$G$2,2,FALSE)</f>
         <v>THU</v>
       </c>
       <c r="C37" t="s">
@@ -1224,7 +1308,7 @@
         <v>41824</v>
       </c>
       <c r="B38" s="9" t="str">
-        <f>HLOOKUP(WEEKDAY(A38),Sheet1!$A$1:$G$2,2,FALSE)</f>
+        <f>HLOOKUP(WEEKDAY(A38),Constants!$A$1:$G$2,2,FALSE)</f>
         <v>FRI</v>
       </c>
       <c r="C38" t="s">
@@ -1239,7 +1323,7 @@
         <v>41825</v>
       </c>
       <c r="B39" s="9" t="str">
-        <f>HLOOKUP(WEEKDAY(A39),Sheet1!$A$1:$G$2,2,FALSE)</f>
+        <f>HLOOKUP(WEEKDAY(A39),Constants!$A$1:$G$2,2,FALSE)</f>
         <v>SAT</v>
       </c>
       <c r="C39" s="6" t="s">
@@ -1259,7 +1343,7 @@
         <v>41826</v>
       </c>
       <c r="B40" s="9" t="str">
-        <f>HLOOKUP(WEEKDAY(A40),Sheet1!$A$1:$G$2,2,FALSE)</f>
+        <f>HLOOKUP(WEEKDAY(A40),Constants!$A$1:$G$2,2,FALSE)</f>
         <v>SUN</v>
       </c>
       <c r="C40" s="6" t="s">
@@ -1279,7 +1363,7 @@
         <v>41827</v>
       </c>
       <c r="B41" s="9" t="str">
-        <f>HLOOKUP(WEEKDAY(A41),Sheet1!$A$1:$G$2,2,FALSE)</f>
+        <f>HLOOKUP(WEEKDAY(A41),Constants!$A$1:$G$2,2,FALSE)</f>
         <v>MON</v>
       </c>
       <c r="C41" t="s">
@@ -1294,7 +1378,7 @@
         <v>41828</v>
       </c>
       <c r="B42" s="9" t="str">
-        <f>HLOOKUP(WEEKDAY(A42),Sheet1!$A$1:$G$2,2,FALSE)</f>
+        <f>HLOOKUP(WEEKDAY(A42),Constants!$A$1:$G$2,2,FALSE)</f>
         <v>TUE</v>
       </c>
       <c r="C42" t="s">
@@ -1309,7 +1393,7 @@
         <v>41829</v>
       </c>
       <c r="B43" s="9" t="str">
-        <f>HLOOKUP(WEEKDAY(A43),Sheet1!$A$1:$G$2,2,FALSE)</f>
+        <f>HLOOKUP(WEEKDAY(A43),Constants!$A$1:$G$2,2,FALSE)</f>
         <v>WED</v>
       </c>
       <c r="C43" t="s">
@@ -1324,7 +1408,7 @@
         <v>41830</v>
       </c>
       <c r="B44" s="9" t="str">
-        <f>HLOOKUP(WEEKDAY(A44),Sheet1!$A$1:$G$2,2,FALSE)</f>
+        <f>HLOOKUP(WEEKDAY(A44),Constants!$A$1:$G$2,2,FALSE)</f>
         <v>THU</v>
       </c>
       <c r="C44" t="s">
@@ -1339,7 +1423,7 @@
         <v>41831</v>
       </c>
       <c r="B45" s="9" t="str">
-        <f>HLOOKUP(WEEKDAY(A45),Sheet1!$A$1:$G$2,2,FALSE)</f>
+        <f>HLOOKUP(WEEKDAY(A45),Constants!$A$1:$G$2,2,FALSE)</f>
         <v>FRI</v>
       </c>
       <c r="D45">
@@ -1351,7 +1435,7 @@
         <v>41832</v>
       </c>
       <c r="B46" s="9" t="str">
-        <f>HLOOKUP(WEEKDAY(A46),Sheet1!$A$1:$G$2,2,FALSE)</f>
+        <f>HLOOKUP(WEEKDAY(A46),Constants!$A$1:$G$2,2,FALSE)</f>
         <v>SAT</v>
       </c>
       <c r="C46" s="6" t="s">
@@ -1371,7 +1455,7 @@
         <v>41833</v>
       </c>
       <c r="B47" s="9" t="str">
-        <f>HLOOKUP(WEEKDAY(A47),Sheet1!$A$1:$G$2,2,FALSE)</f>
+        <f>HLOOKUP(WEEKDAY(A47),Constants!$A$1:$G$2,2,FALSE)</f>
         <v>SUN</v>
       </c>
       <c r="C47" s="6" t="s">
@@ -1391,7 +1475,7 @@
         <v>41834</v>
       </c>
       <c r="B48" s="9" t="str">
-        <f>HLOOKUP(WEEKDAY(A48),Sheet1!$A$1:$G$2,2,FALSE)</f>
+        <f>HLOOKUP(WEEKDAY(A48),Constants!$A$1:$G$2,2,FALSE)</f>
         <v>MON</v>
       </c>
       <c r="C48" t="s">
@@ -1406,7 +1490,7 @@
         <v>41835</v>
       </c>
       <c r="B49" s="9" t="str">
-        <f>HLOOKUP(WEEKDAY(A49),Sheet1!$A$1:$G$2,2,FALSE)</f>
+        <f>HLOOKUP(WEEKDAY(A49),Constants!$A$1:$G$2,2,FALSE)</f>
         <v>TUE</v>
       </c>
       <c r="C49" t="s">
@@ -1421,7 +1505,7 @@
         <v>41836</v>
       </c>
       <c r="B50" s="9" t="str">
-        <f>HLOOKUP(WEEKDAY(A50),Sheet1!$A$1:$G$2,2,FALSE)</f>
+        <f>HLOOKUP(WEEKDAY(A50),Constants!$A$1:$G$2,2,FALSE)</f>
         <v>WED</v>
       </c>
       <c r="C50" t="s">
@@ -1436,7 +1520,7 @@
         <v>41837</v>
       </c>
       <c r="B51" s="9" t="str">
-        <f>HLOOKUP(WEEKDAY(A51),Sheet1!$A$1:$G$2,2,FALSE)</f>
+        <f>HLOOKUP(WEEKDAY(A51),Constants!$A$1:$G$2,2,FALSE)</f>
         <v>THU</v>
       </c>
       <c r="C51" t="s">
@@ -1451,7 +1535,7 @@
         <v>41838</v>
       </c>
       <c r="B52" s="9" t="str">
-        <f>HLOOKUP(WEEKDAY(A52),Sheet1!$A$1:$G$2,2,FALSE)</f>
+        <f>HLOOKUP(WEEKDAY(A52),Constants!$A$1:$G$2,2,FALSE)</f>
         <v>FRI</v>
       </c>
       <c r="C52" t="s">
@@ -1466,7 +1550,7 @@
         <v>41839</v>
       </c>
       <c r="B53" s="9" t="str">
-        <f>HLOOKUP(WEEKDAY(A53),Sheet1!$A$1:$G$2,2,FALSE)</f>
+        <f>HLOOKUP(WEEKDAY(A53),Constants!$A$1:$G$2,2,FALSE)</f>
         <v>SAT</v>
       </c>
       <c r="C53" t="s">
@@ -1481,7 +1565,7 @@
         <v>41841</v>
       </c>
       <c r="B54" s="9" t="str">
-        <f>HLOOKUP(WEEKDAY(A54),Sheet1!$A$1:$G$2,2,FALSE)</f>
+        <f>HLOOKUP(WEEKDAY(A54),Constants!$A$1:$G$2,2,FALSE)</f>
         <v>MON</v>
       </c>
       <c r="C54" t="s">
@@ -1496,7 +1580,7 @@
         <v>41842</v>
       </c>
       <c r="B55" s="9" t="str">
-        <f>HLOOKUP(WEEKDAY(A55),Sheet1!$A$1:$G$2,2,FALSE)</f>
+        <f>HLOOKUP(WEEKDAY(A55),Constants!$A$1:$G$2,2,FALSE)</f>
         <v>TUE</v>
       </c>
       <c r="C55" t="s">
@@ -1511,7 +1595,7 @@
         <v>41843</v>
       </c>
       <c r="B56" s="9" t="str">
-        <f>HLOOKUP(WEEKDAY(A56),Sheet1!$A$1:$G$2,2,FALSE)</f>
+        <f>HLOOKUP(WEEKDAY(A56),Constants!$A$1:$G$2,2,FALSE)</f>
         <v>WED</v>
       </c>
       <c r="C56" t="s">
@@ -1526,7 +1610,7 @@
         <v>41844</v>
       </c>
       <c r="B57" s="9" t="str">
-        <f>HLOOKUP(WEEKDAY(A57),Sheet1!$A$1:$G$2,2,FALSE)</f>
+        <f>HLOOKUP(WEEKDAY(A57),Constants!$A$1:$G$2,2,FALSE)</f>
         <v>THU</v>
       </c>
       <c r="C57" t="s">
@@ -1541,7 +1625,7 @@
         <v>41845</v>
       </c>
       <c r="B58" s="9" t="str">
-        <f>HLOOKUP(WEEKDAY(A58),Sheet1!$A$1:$G$2,2,FALSE)</f>
+        <f>HLOOKUP(WEEKDAY(A58),Constants!$A$1:$G$2,2,FALSE)</f>
         <v>FRI</v>
       </c>
       <c r="C58" t="s">
@@ -1556,7 +1640,7 @@
         <v>41846</v>
       </c>
       <c r="B59" s="9" t="str">
-        <f>HLOOKUP(WEEKDAY(A59),Sheet1!$A$1:$G$2,2,FALSE)</f>
+        <f>HLOOKUP(WEEKDAY(A59),Constants!$A$1:$G$2,2,FALSE)</f>
         <v>SAT</v>
       </c>
     </row>
@@ -1565,7 +1649,7 @@
         <v>41847</v>
       </c>
       <c r="B60" s="9" t="str">
-        <f>HLOOKUP(WEEKDAY(A60),Sheet1!$A$1:$G$2,2,FALSE)</f>
+        <f>HLOOKUP(WEEKDAY(A60),Constants!$A$1:$G$2,2,FALSE)</f>
         <v>SUN</v>
       </c>
       <c r="C60" t="s">
@@ -1580,7 +1664,7 @@
         <v>41848</v>
       </c>
       <c r="B61" s="9" t="str">
-        <f>HLOOKUP(WEEKDAY(A61),Sheet1!$A$1:$G$2,2,FALSE)</f>
+        <f>HLOOKUP(WEEKDAY(A61),Constants!$A$1:$G$2,2,FALSE)</f>
         <v>MON</v>
       </c>
       <c r="C61" t="s">
@@ -1595,7 +1679,7 @@
         <v>41849</v>
       </c>
       <c r="B62" s="9" t="str">
-        <f>HLOOKUP(WEEKDAY(A62),Sheet1!$A$1:$G$2,2,FALSE)</f>
+        <f>HLOOKUP(WEEKDAY(A62),Constants!$A$1:$G$2,2,FALSE)</f>
         <v>TUE</v>
       </c>
       <c r="C62" t="s">
@@ -1610,7 +1694,7 @@
         <v>41850</v>
       </c>
       <c r="B63" s="9" t="str">
-        <f>HLOOKUP(WEEKDAY(A63),Sheet1!$A$1:$G$2,2,FALSE)</f>
+        <f>HLOOKUP(WEEKDAY(A63),Constants!$A$1:$G$2,2,FALSE)</f>
         <v>WED</v>
       </c>
       <c r="C63" t="s">
@@ -1625,7 +1709,7 @@
         <v>41851</v>
       </c>
       <c r="B64" s="9" t="str">
-        <f>HLOOKUP(WEEKDAY(A64),Sheet1!$A$1:$G$2,2,FALSE)</f>
+        <f>HLOOKUP(WEEKDAY(A64),Constants!$A$1:$G$2,2,FALSE)</f>
         <v>THU</v>
       </c>
       <c r="C64" t="s">
@@ -1640,7 +1724,7 @@
         <v>41852</v>
       </c>
       <c r="B65" s="9" t="str">
-        <f>HLOOKUP(WEEKDAY(A65),Sheet1!$A$1:$G$2,2,FALSE)</f>
+        <f>HLOOKUP(WEEKDAY(A65),Constants!$A$1:$G$2,2,FALSE)</f>
         <v>FRI</v>
       </c>
       <c r="C65" t="s">
@@ -1655,7 +1739,7 @@
         <v>41853</v>
       </c>
       <c r="B66" s="9" t="str">
-        <f>HLOOKUP(WEEKDAY(A66),Sheet1!$A$1:$G$2,2,FALSE)</f>
+        <f>HLOOKUP(WEEKDAY(A66),Constants!$A$1:$G$2,2,FALSE)</f>
         <v>SAT</v>
       </c>
       <c r="C66" t="s">
@@ -1670,7 +1754,7 @@
         <v>41854</v>
       </c>
       <c r="B67" s="9" t="str">
-        <f>HLOOKUP(WEEKDAY(A67),Sheet1!$A$1:$G$2,2,FALSE)</f>
+        <f>HLOOKUP(WEEKDAY(A67),Constants!$A$1:$G$2,2,FALSE)</f>
         <v>SUN</v>
       </c>
       <c r="C67" t="s">
@@ -1685,7 +1769,7 @@
         <v>41855</v>
       </c>
       <c r="B68" s="9" t="str">
-        <f>HLOOKUP(WEEKDAY(A68),Sheet1!$A$1:$G$2,2,FALSE)</f>
+        <f>HLOOKUP(WEEKDAY(A68),Constants!$A$1:$G$2,2,FALSE)</f>
         <v>MON</v>
       </c>
       <c r="C68" t="s">
@@ -1700,7 +1784,7 @@
         <v>41856</v>
       </c>
       <c r="B69" s="9" t="str">
-        <f>HLOOKUP(WEEKDAY(A69),Sheet1!$A$1:$G$2,2,FALSE)</f>
+        <f>HLOOKUP(WEEKDAY(A69),Constants!$A$1:$G$2,2,FALSE)</f>
         <v>TUE</v>
       </c>
       <c r="C69" t="s">
@@ -1715,7 +1799,7 @@
         <v>41857</v>
       </c>
       <c r="B70" s="9" t="str">
-        <f>HLOOKUP(WEEKDAY(A70),Sheet1!$A$1:$G$2,2,FALSE)</f>
+        <f>HLOOKUP(WEEKDAY(A70),Constants!$A$1:$G$2,2,FALSE)</f>
         <v>WED</v>
       </c>
       <c r="C70" t="s">
@@ -1730,7 +1814,7 @@
         <v>41858</v>
       </c>
       <c r="B71" s="9" t="str">
-        <f>HLOOKUP(WEEKDAY(A71),Sheet1!$A$1:$G$2,2,FALSE)</f>
+        <f>HLOOKUP(WEEKDAY(A71),Constants!$A$1:$G$2,2,FALSE)</f>
         <v>THU</v>
       </c>
       <c r="C71" t="s">
@@ -1745,7 +1829,7 @@
         <v>41859</v>
       </c>
       <c r="B72" s="9" t="str">
-        <f>HLOOKUP(WEEKDAY(A72),Sheet1!$A$1:$G$2,2,FALSE)</f>
+        <f>HLOOKUP(WEEKDAY(A72),Constants!$A$1:$G$2,2,FALSE)</f>
         <v>FRI</v>
       </c>
       <c r="C72" t="s">
@@ -1760,7 +1844,7 @@
         <v>41860</v>
       </c>
       <c r="B73" s="9" t="str">
-        <f>HLOOKUP(WEEKDAY(A73),Sheet1!$A$1:$G$2,2,FALSE)</f>
+        <f>HLOOKUP(WEEKDAY(A73),Constants!$A$1:$G$2,2,FALSE)</f>
         <v>SAT</v>
       </c>
       <c r="D73">
@@ -1772,7 +1856,7 @@
         <v>41861</v>
       </c>
       <c r="B74" s="9" t="str">
-        <f>HLOOKUP(WEEKDAY(A74),Sheet1!$A$1:$G$2,2,FALSE)</f>
+        <f>HLOOKUP(WEEKDAY(A74),Constants!$A$1:$G$2,2,FALSE)</f>
         <v>SUN</v>
       </c>
       <c r="D74">
@@ -1784,7 +1868,7 @@
         <v>41862</v>
       </c>
       <c r="B75" s="9" t="str">
-        <f>HLOOKUP(WEEKDAY(A75),Sheet1!$A$1:$G$2,2,FALSE)</f>
+        <f>HLOOKUP(WEEKDAY(A75),Constants!$A$1:$G$2,2,FALSE)</f>
         <v>MON</v>
       </c>
       <c r="D75">
@@ -1796,7 +1880,7 @@
         <v>41863</v>
       </c>
       <c r="B76" s="9" t="str">
-        <f>HLOOKUP(WEEKDAY(A76),Sheet1!$A$1:$G$2,2,FALSE)</f>
+        <f>HLOOKUP(WEEKDAY(A76),Constants!$A$1:$G$2,2,FALSE)</f>
         <v>TUE</v>
       </c>
       <c r="D76">
@@ -1808,7 +1892,7 @@
         <v>41864</v>
       </c>
       <c r="B77" s="9" t="str">
-        <f>HLOOKUP(WEEKDAY(A77),Sheet1!$A$1:$G$2,2,FALSE)</f>
+        <f>HLOOKUP(WEEKDAY(A77),Constants!$A$1:$G$2,2,FALSE)</f>
         <v>WED</v>
       </c>
       <c r="D77">
@@ -1820,7 +1904,7 @@
         <v>41865</v>
       </c>
       <c r="B78" s="9" t="str">
-        <f>HLOOKUP(WEEKDAY(A78),Sheet1!$A$1:$G$2,2,FALSE)</f>
+        <f>HLOOKUP(WEEKDAY(A78),Constants!$A$1:$G$2,2,FALSE)</f>
         <v>THU</v>
       </c>
       <c r="D78">
@@ -1832,7 +1916,7 @@
         <v>41866</v>
       </c>
       <c r="B79" s="9" t="str">
-        <f>HLOOKUP(WEEKDAY(A79),Sheet1!$A$1:$G$2,2,FALSE)</f>
+        <f>HLOOKUP(WEEKDAY(A79),Constants!$A$1:$G$2,2,FALSE)</f>
         <v>FRI</v>
       </c>
       <c r="D79">
@@ -1844,7 +1928,7 @@
         <v>41867</v>
       </c>
       <c r="B80" s="9" t="str">
-        <f>HLOOKUP(WEEKDAY(A80),Sheet1!$A$1:$G$2,2,FALSE)</f>
+        <f>HLOOKUP(WEEKDAY(A80),Constants!$A$1:$G$2,2,FALSE)</f>
         <v>SAT</v>
       </c>
       <c r="D80">
@@ -1856,7 +1940,7 @@
         <v>41868</v>
       </c>
       <c r="B81" s="9" t="str">
-        <f>HLOOKUP(WEEKDAY(A81),Sheet1!$A$1:$G$2,2,FALSE)</f>
+        <f>HLOOKUP(WEEKDAY(A81),Constants!$A$1:$G$2,2,FALSE)</f>
         <v>SUN</v>
       </c>
       <c r="D81">
@@ -1868,7 +1952,7 @@
         <v>41869</v>
       </c>
       <c r="B82" s="9" t="str">
-        <f>HLOOKUP(WEEKDAY(A82),Sheet1!$A$1:$G$2,2,FALSE)</f>
+        <f>HLOOKUP(WEEKDAY(A82),Constants!$A$1:$G$2,2,FALSE)</f>
         <v>MON</v>
       </c>
       <c r="D82">
@@ -1880,7 +1964,7 @@
         <v>41870</v>
       </c>
       <c r="B83" s="9" t="str">
-        <f>HLOOKUP(WEEKDAY(A83),Sheet1!$A$1:$G$2,2,FALSE)</f>
+        <f>HLOOKUP(WEEKDAY(A83),Constants!$A$1:$G$2,2,FALSE)</f>
         <v>TUE</v>
       </c>
       <c r="D83">
@@ -1892,7 +1976,7 @@
         <v>41871</v>
       </c>
       <c r="B84" s="9" t="str">
-        <f>HLOOKUP(WEEKDAY(A84),Sheet1!$A$1:$G$2,2,FALSE)</f>
+        <f>HLOOKUP(WEEKDAY(A84),Constants!$A$1:$G$2,2,FALSE)</f>
         <v>WED</v>
       </c>
       <c r="D84">
@@ -1904,7 +1988,7 @@
         <v>41872</v>
       </c>
       <c r="B85" s="9" t="str">
-        <f>HLOOKUP(WEEKDAY(A85),Sheet1!$A$1:$G$2,2,FALSE)</f>
+        <f>HLOOKUP(WEEKDAY(A85),Constants!$A$1:$G$2,2,FALSE)</f>
         <v>THU</v>
       </c>
       <c r="D85">
@@ -1916,7 +2000,7 @@
         <v>41873</v>
       </c>
       <c r="B86" s="9" t="str">
-        <f>HLOOKUP(WEEKDAY(A86),Sheet1!$A$1:$G$2,2,FALSE)</f>
+        <f>HLOOKUP(WEEKDAY(A86),Constants!$A$1:$G$2,2,FALSE)</f>
         <v>FRI</v>
       </c>
       <c r="D86">
@@ -1928,7 +2012,7 @@
         <v>41874</v>
       </c>
       <c r="B87" s="9" t="str">
-        <f>HLOOKUP(WEEKDAY(A87),Sheet1!$A$1:$G$2,2,FALSE)</f>
+        <f>HLOOKUP(WEEKDAY(A87),Constants!$A$1:$G$2,2,FALSE)</f>
         <v>SAT</v>
       </c>
       <c r="D87">
@@ -1940,7 +2024,7 @@
         <v>41875</v>
       </c>
       <c r="B88" s="9" t="str">
-        <f>HLOOKUP(WEEKDAY(A88),Sheet1!$A$1:$G$2,2,FALSE)</f>
+        <f>HLOOKUP(WEEKDAY(A88),Constants!$A$1:$G$2,2,FALSE)</f>
         <v>SUN</v>
       </c>
       <c r="D88">
@@ -1952,7 +2036,7 @@
         <v>41876</v>
       </c>
       <c r="B89" s="9" t="str">
-        <f>HLOOKUP(WEEKDAY(A89),Sheet1!$A$1:$G$2,2,FALSE)</f>
+        <f>HLOOKUP(WEEKDAY(A89),Constants!$A$1:$G$2,2,FALSE)</f>
         <v>MON</v>
       </c>
       <c r="D89">
@@ -1964,7 +2048,7 @@
         <v>41877</v>
       </c>
       <c r="B90" s="9" t="str">
-        <f>HLOOKUP(WEEKDAY(A90),Sheet1!$A$1:$G$2,2,FALSE)</f>
+        <f>HLOOKUP(WEEKDAY(A90),Constants!$A$1:$G$2,2,FALSE)</f>
         <v>TUE</v>
       </c>
       <c r="D90">
@@ -1976,7 +2060,7 @@
         <v>41878</v>
       </c>
       <c r="B91" s="9" t="str">
-        <f>HLOOKUP(WEEKDAY(A91),Sheet1!$A$1:$G$2,2,FALSE)</f>
+        <f>HLOOKUP(WEEKDAY(A91),Constants!$A$1:$G$2,2,FALSE)</f>
         <v>WED</v>
       </c>
       <c r="D91">
@@ -1988,7 +2072,7 @@
         <v>41879</v>
       </c>
       <c r="B92" s="9" t="str">
-        <f>HLOOKUP(WEEKDAY(A92),Sheet1!$A$1:$G$2,2,FALSE)</f>
+        <f>HLOOKUP(WEEKDAY(A92),Constants!$A$1:$G$2,2,FALSE)</f>
         <v>THU</v>
       </c>
       <c r="D92">
@@ -2000,7 +2084,7 @@
         <v>41880</v>
       </c>
       <c r="B93" s="9" t="str">
-        <f>HLOOKUP(WEEKDAY(A93),Sheet1!$A$1:$G$2,2,FALSE)</f>
+        <f>HLOOKUP(WEEKDAY(A93),Constants!$A$1:$G$2,2,FALSE)</f>
         <v>FRI</v>
       </c>
       <c r="D93">
@@ -2012,7 +2096,7 @@
         <v>41881</v>
       </c>
       <c r="B94" s="9" t="str">
-        <f>HLOOKUP(WEEKDAY(A94),Sheet1!$A$1:$G$2,2,FALSE)</f>
+        <f>HLOOKUP(WEEKDAY(A94),Constants!$A$1:$G$2,2,FALSE)</f>
         <v>SAT</v>
       </c>
       <c r="D94">
@@ -2024,7 +2108,7 @@
         <v>41882</v>
       </c>
       <c r="B95" s="9" t="str">
-        <f>HLOOKUP(WEEKDAY(A95),Sheet1!$A$1:$G$2,2,FALSE)</f>
+        <f>HLOOKUP(WEEKDAY(A95),Constants!$A$1:$G$2,2,FALSE)</f>
         <v>SUN</v>
       </c>
       <c r="D95">
@@ -2036,7 +2120,7 @@
         <v>41883</v>
       </c>
       <c r="B96" s="9" t="str">
-        <f>HLOOKUP(WEEKDAY(A96),Sheet1!$A$1:$G$2,2,FALSE)</f>
+        <f>HLOOKUP(WEEKDAY(A96),Constants!$A$1:$G$2,2,FALSE)</f>
         <v>MON</v>
       </c>
       <c r="D96">
@@ -2048,7 +2132,7 @@
         <v>41884</v>
       </c>
       <c r="B97" s="9" t="str">
-        <f>HLOOKUP(WEEKDAY(A97),Sheet1!$A$1:$G$2,2,FALSE)</f>
+        <f>HLOOKUP(WEEKDAY(A97),Constants!$A$1:$G$2,2,FALSE)</f>
         <v>TUE</v>
       </c>
       <c r="D97">
@@ -2060,7 +2144,7 @@
         <v>41885</v>
       </c>
       <c r="B98" s="9" t="str">
-        <f>HLOOKUP(WEEKDAY(A98),Sheet1!$A$1:$G$2,2,FALSE)</f>
+        <f>HLOOKUP(WEEKDAY(A98),Constants!$A$1:$G$2,2,FALSE)</f>
         <v>WED</v>
       </c>
       <c r="D98">
@@ -2072,7 +2156,7 @@
         <v>41886</v>
       </c>
       <c r="B99" s="9" t="str">
-        <f>HLOOKUP(WEEKDAY(A99),Sheet1!$A$1:$G$2,2,FALSE)</f>
+        <f>HLOOKUP(WEEKDAY(A99),Constants!$A$1:$G$2,2,FALSE)</f>
         <v>THU</v>
       </c>
       <c r="D99">
@@ -2084,7 +2168,7 @@
         <v>41887</v>
       </c>
       <c r="B100" s="9" t="str">
-        <f>HLOOKUP(WEEKDAY(A100),Sheet1!$A$1:$G$2,2,FALSE)</f>
+        <f>HLOOKUP(WEEKDAY(A100),Constants!$A$1:$G$2,2,FALSE)</f>
         <v>FRI</v>
       </c>
       <c r="D100">
@@ -2096,7 +2180,7 @@
         <v>41888</v>
       </c>
       <c r="B101" s="9" t="str">
-        <f>HLOOKUP(WEEKDAY(A101),Sheet1!$A$1:$G$2,2,FALSE)</f>
+        <f>HLOOKUP(WEEKDAY(A101),Constants!$A$1:$G$2,2,FALSE)</f>
         <v>SAT</v>
       </c>
       <c r="D101">
@@ -2108,7 +2192,7 @@
         <v>41889</v>
       </c>
       <c r="B102" s="9" t="str">
-        <f>HLOOKUP(WEEKDAY(A102),Sheet1!$A$1:$G$2,2,FALSE)</f>
+        <f>HLOOKUP(WEEKDAY(A102),Constants!$A$1:$G$2,2,FALSE)</f>
         <v>SUN</v>
       </c>
       <c r="D102">
@@ -2120,7 +2204,7 @@
         <v>41890</v>
       </c>
       <c r="B103" s="9" t="str">
-        <f>HLOOKUP(WEEKDAY(A103),Sheet1!$A$1:$G$2,2,FALSE)</f>
+        <f>HLOOKUP(WEEKDAY(A103),Constants!$A$1:$G$2,2,FALSE)</f>
         <v>MON</v>
       </c>
       <c r="D103">
@@ -2132,7 +2216,7 @@
         <v>41891</v>
       </c>
       <c r="B104" s="9" t="str">
-        <f>HLOOKUP(WEEKDAY(A104),Sheet1!$A$1:$G$2,2,FALSE)</f>
+        <f>HLOOKUP(WEEKDAY(A104),Constants!$A$1:$G$2,2,FALSE)</f>
         <v>TUE</v>
       </c>
       <c r="D104">
@@ -2144,7 +2228,7 @@
         <v>41892</v>
       </c>
       <c r="B105" s="9" t="str">
-        <f>HLOOKUP(WEEKDAY(A105),Sheet1!$A$1:$G$2,2,FALSE)</f>
+        <f>HLOOKUP(WEEKDAY(A105),Constants!$A$1:$G$2,2,FALSE)</f>
         <v>WED</v>
       </c>
       <c r="D105">
@@ -2156,7 +2240,7 @@
         <v>41893</v>
       </c>
       <c r="B106" s="9" t="str">
-        <f>HLOOKUP(WEEKDAY(A106),Sheet1!$A$1:$G$2,2,FALSE)</f>
+        <f>HLOOKUP(WEEKDAY(A106),Constants!$A$1:$G$2,2,FALSE)</f>
         <v>THU</v>
       </c>
       <c r="D106">
@@ -2168,7 +2252,7 @@
         <v>41894</v>
       </c>
       <c r="B107" s="9" t="str">
-        <f>HLOOKUP(WEEKDAY(A107),Sheet1!$A$1:$G$2,2,FALSE)</f>
+        <f>HLOOKUP(WEEKDAY(A107),Constants!$A$1:$G$2,2,FALSE)</f>
         <v>FRI</v>
       </c>
       <c r="D107">
@@ -2180,7 +2264,7 @@
         <v>41895</v>
       </c>
       <c r="B108" s="9" t="str">
-        <f>HLOOKUP(WEEKDAY(A108),Sheet1!$A$1:$G$2,2,FALSE)</f>
+        <f>HLOOKUP(WEEKDAY(A108),Constants!$A$1:$G$2,2,FALSE)</f>
         <v>SAT</v>
       </c>
       <c r="D108">
@@ -2192,7 +2276,7 @@
         <v>41896</v>
       </c>
       <c r="B109" s="9" t="str">
-        <f>HLOOKUP(WEEKDAY(A109),Sheet1!$A$1:$G$2,2,FALSE)</f>
+        <f>HLOOKUP(WEEKDAY(A109),Constants!$A$1:$G$2,2,FALSE)</f>
         <v>SUN</v>
       </c>
       <c r="D109">
@@ -2204,7 +2288,7 @@
         <v>41897</v>
       </c>
       <c r="B110" s="9" t="str">
-        <f>HLOOKUP(WEEKDAY(A110),Sheet1!$A$1:$G$2,2,FALSE)</f>
+        <f>HLOOKUP(WEEKDAY(A110),Constants!$A$1:$G$2,2,FALSE)</f>
         <v>MON</v>
       </c>
       <c r="D110">
@@ -2216,7 +2300,7 @@
         <v>41898</v>
       </c>
       <c r="B111" s="9" t="str">
-        <f>HLOOKUP(WEEKDAY(A111),Sheet1!$A$1:$G$2,2,FALSE)</f>
+        <f>HLOOKUP(WEEKDAY(A111),Constants!$A$1:$G$2,2,FALSE)</f>
         <v>TUE</v>
       </c>
       <c r="D111">
@@ -2228,11 +2312,389 @@
         <v>41899</v>
       </c>
       <c r="B112" s="9" t="str">
-        <f>HLOOKUP(WEEKDAY(A112),Sheet1!$A$1:$G$2,2,FALSE)</f>
+        <f>HLOOKUP(WEEKDAY(A112),Constants!$A$1:$G$2,2,FALSE)</f>
         <v>WED</v>
       </c>
       <c r="D112">
         <v>4</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A113" s="1">
+        <v>41900</v>
+      </c>
+      <c r="B113" s="9" t="str">
+        <f>HLOOKUP(WEEKDAY(A113),Constants!$A$1:$G$2,2,FALSE)</f>
+        <v>THU</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A114" s="1">
+        <v>41901</v>
+      </c>
+      <c r="B114" s="9" t="str">
+        <f>HLOOKUP(WEEKDAY(A114),Constants!$A$1:$G$2,2,FALSE)</f>
+        <v>FRI</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A115" s="1">
+        <v>41902</v>
+      </c>
+      <c r="B115" s="9" t="str">
+        <f>HLOOKUP(WEEKDAY(A115),Constants!$A$1:$G$2,2,FALSE)</f>
+        <v>SAT</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A116" s="1">
+        <v>41903</v>
+      </c>
+      <c r="B116" s="9" t="str">
+        <f>HLOOKUP(WEEKDAY(A116),Constants!$A$1:$G$2,2,FALSE)</f>
+        <v>SUN</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A117" s="1">
+        <v>41904</v>
+      </c>
+      <c r="B117" s="9" t="str">
+        <f>HLOOKUP(WEEKDAY(A117),Constants!$A$1:$G$2,2,FALSE)</f>
+        <v>MON</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A118" s="1">
+        <v>41905</v>
+      </c>
+      <c r="B118" s="9" t="str">
+        <f>HLOOKUP(WEEKDAY(A118),Constants!$A$1:$G$2,2,FALSE)</f>
+        <v>TUE</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A119" s="1">
+        <v>41906</v>
+      </c>
+      <c r="B119" s="9" t="str">
+        <f>HLOOKUP(WEEKDAY(A119),Constants!$A$1:$G$2,2,FALSE)</f>
+        <v>WED</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A120" s="1">
+        <v>41907</v>
+      </c>
+      <c r="B120" s="9" t="str">
+        <f>HLOOKUP(WEEKDAY(A120),Constants!$A$1:$G$2,2,FALSE)</f>
+        <v>THU</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A121" s="1">
+        <v>41908</v>
+      </c>
+      <c r="B121" s="9" t="str">
+        <f>HLOOKUP(WEEKDAY(A121),Constants!$A$1:$G$2,2,FALSE)</f>
+        <v>FRI</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A122" s="1">
+        <v>41909</v>
+      </c>
+      <c r="B122" s="9" t="str">
+        <f>HLOOKUP(WEEKDAY(A122),Constants!$A$1:$G$2,2,FALSE)</f>
+        <v>SAT</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A123" s="1">
+        <v>41910</v>
+      </c>
+      <c r="B123" s="9" t="str">
+        <f>HLOOKUP(WEEKDAY(A123),Constants!$A$1:$G$2,2,FALSE)</f>
+        <v>SUN</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A124" s="1">
+        <v>41911</v>
+      </c>
+      <c r="B124" s="9" t="str">
+        <f>HLOOKUP(WEEKDAY(A124),Constants!$A$1:$G$2,2,FALSE)</f>
+        <v>MON</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A125" s="1">
+        <v>41912</v>
+      </c>
+      <c r="B125" s="9" t="str">
+        <f>HLOOKUP(WEEKDAY(A125),Constants!$A$1:$G$2,2,FALSE)</f>
+        <v>TUE</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A126" s="1">
+        <v>41913</v>
+      </c>
+      <c r="B126" s="9" t="str">
+        <f>HLOOKUP(WEEKDAY(A126),Constants!$A$1:$G$2,2,FALSE)</f>
+        <v>WED</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A127" s="1">
+        <v>41914</v>
+      </c>
+      <c r="B127" s="9" t="str">
+        <f>HLOOKUP(WEEKDAY(A127),Constants!$A$1:$G$2,2,FALSE)</f>
+        <v>THU</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A128" s="1">
+        <v>41915</v>
+      </c>
+      <c r="B128" s="9" t="str">
+        <f>HLOOKUP(WEEKDAY(A128),Constants!$A$1:$G$2,2,FALSE)</f>
+        <v>FRI</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A129" s="1">
+        <v>41916</v>
+      </c>
+      <c r="B129" s="9" t="str">
+        <f>HLOOKUP(WEEKDAY(A129),Constants!$A$1:$G$2,2,FALSE)</f>
+        <v>SAT</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A130" s="1">
+        <v>41917</v>
+      </c>
+      <c r="B130" s="9" t="str">
+        <f>HLOOKUP(WEEKDAY(A130),Constants!$A$1:$G$2,2,FALSE)</f>
+        <v>SUN</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A131" s="1">
+        <v>41918</v>
+      </c>
+      <c r="B131" s="9" t="str">
+        <f>HLOOKUP(WEEKDAY(A131),Constants!$A$1:$G$2,2,FALSE)</f>
+        <v>MON</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A132" s="1">
+        <v>41919</v>
+      </c>
+      <c r="B132" s="9" t="str">
+        <f>HLOOKUP(WEEKDAY(A132),Constants!$A$1:$G$2,2,FALSE)</f>
+        <v>TUE</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A133" s="1">
+        <v>41920</v>
+      </c>
+      <c r="B133" s="9" t="str">
+        <f>HLOOKUP(WEEKDAY(A133),Constants!$A$1:$G$2,2,FALSE)</f>
+        <v>WED</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A134" s="1">
+        <v>41921</v>
+      </c>
+      <c r="B134" s="9" t="str">
+        <f>HLOOKUP(WEEKDAY(A134),Constants!$A$1:$G$2,2,FALSE)</f>
+        <v>THU</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A135" s="1">
+        <v>41922</v>
+      </c>
+      <c r="B135" s="9" t="str">
+        <f>HLOOKUP(WEEKDAY(A135),Constants!$A$1:$G$2,2,FALSE)</f>
+        <v>FRI</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A136" s="1">
+        <v>41923</v>
+      </c>
+      <c r="B136" s="9" t="str">
+        <f>HLOOKUP(WEEKDAY(A136),Constants!$A$1:$G$2,2,FALSE)</f>
+        <v>SAT</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A137" s="1">
+        <v>41924</v>
+      </c>
+      <c r="B137" s="9" t="str">
+        <f>HLOOKUP(WEEKDAY(A137),Constants!$A$1:$G$2,2,FALSE)</f>
+        <v>SUN</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A138" s="1">
+        <v>41925</v>
+      </c>
+      <c r="B138" s="9" t="str">
+        <f>HLOOKUP(WEEKDAY(A138),Constants!$A$1:$G$2,2,FALSE)</f>
+        <v>MON</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A139" s="1">
+        <v>41926</v>
+      </c>
+      <c r="B139" s="9" t="str">
+        <f>HLOOKUP(WEEKDAY(A139),Constants!$A$1:$G$2,2,FALSE)</f>
+        <v>TUE</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A140" s="1">
+        <v>41927</v>
+      </c>
+      <c r="B140" s="9" t="str">
+        <f>HLOOKUP(WEEKDAY(A140),Constants!$A$1:$G$2,2,FALSE)</f>
+        <v>WED</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A141" s="1">
+        <v>41928</v>
+      </c>
+      <c r="B141" s="9" t="str">
+        <f>HLOOKUP(WEEKDAY(A141),Constants!$A$1:$G$2,2,FALSE)</f>
+        <v>THU</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A142" s="1">
+        <v>41929</v>
+      </c>
+      <c r="B142" s="9" t="str">
+        <f>HLOOKUP(WEEKDAY(A142),Constants!$A$1:$G$2,2,FALSE)</f>
+        <v>FRI</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A143" s="1">
+        <v>41930</v>
+      </c>
+      <c r="B143" s="9" t="str">
+        <f>HLOOKUP(WEEKDAY(A143),Constants!$A$1:$G$2,2,FALSE)</f>
+        <v>SAT</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A144" s="1">
+        <v>41931</v>
+      </c>
+      <c r="B144" s="9" t="str">
+        <f>HLOOKUP(WEEKDAY(A144),Constants!$A$1:$G$2,2,FALSE)</f>
+        <v>SUN</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A145" s="1">
+        <v>41932</v>
+      </c>
+      <c r="B145" s="9" t="str">
+        <f>HLOOKUP(WEEKDAY(A145),Constants!$A$1:$G$2,2,FALSE)</f>
+        <v>MON</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A146" s="1">
+        <v>41933</v>
+      </c>
+      <c r="B146" s="9" t="str">
+        <f>HLOOKUP(WEEKDAY(A146),Constants!$A$1:$G$2,2,FALSE)</f>
+        <v>TUE</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A147" s="1">
+        <v>41934</v>
+      </c>
+      <c r="B147" s="9" t="str">
+        <f>HLOOKUP(WEEKDAY(A147),Constants!$A$1:$G$2,2,FALSE)</f>
+        <v>WED</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A148" s="1">
+        <v>41935</v>
+      </c>
+      <c r="B148" s="9" t="str">
+        <f>HLOOKUP(WEEKDAY(A148),Constants!$A$1:$G$2,2,FALSE)</f>
+        <v>THU</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A149" s="1">
+        <v>41936</v>
+      </c>
+      <c r="B149" s="9" t="str">
+        <f>HLOOKUP(WEEKDAY(A149),Constants!$A$1:$G$2,2,FALSE)</f>
+        <v>FRI</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A150" s="1">
+        <v>41937</v>
+      </c>
+      <c r="B150" s="9" t="str">
+        <f>HLOOKUP(WEEKDAY(A150),Constants!$A$1:$G$2,2,FALSE)</f>
+        <v>SAT</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A151" s="1">
+        <v>41938</v>
+      </c>
+      <c r="B151" s="9" t="str">
+        <f>HLOOKUP(WEEKDAY(A151),Constants!$A$1:$G$2,2,FALSE)</f>
+        <v>SUN</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A152" s="1">
+        <v>41939</v>
+      </c>
+      <c r="B152" s="9" t="str">
+        <f>HLOOKUP(WEEKDAY(A152),Constants!$A$1:$G$2,2,FALSE)</f>
+        <v>MON</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A153" s="1">
+        <v>41940</v>
+      </c>
+      <c r="B153" s="9" t="str">
+        <f>HLOOKUP(WEEKDAY(A153),Constants!$A$1:$G$2,2,FALSE)</f>
+        <v>TUE</v>
+      </c>
+    </row>
+    <row r="154" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A154" s="1">
+        <v>41941</v>
+      </c>
+      <c r="B154" s="9" t="str">
+        <f>HLOOKUP(WEEKDAY(A154),Constants!$A$1:$G$2,2,FALSE)</f>
+        <v>WED</v>
       </c>
     </row>
   </sheetData>
@@ -2241,7 +2703,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E8"/>
   <sheetViews>
@@ -2359,63 +2821,51 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A2:C12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.140625" customWidth="1"/>
+    <col min="2" max="2" width="20.5703125" customWidth="1"/>
+    <col min="3" max="3" width="29.7109375" customWidth="1"/>
+    <col min="4" max="4" width="14" customWidth="1"/>
+    <col min="5" max="5" width="15.140625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1">
-        <v>1</v>
-      </c>
-      <c r="B1">
-        <v>2</v>
-      </c>
-      <c r="C1">
-        <v>3</v>
-      </c>
-      <c r="D1">
-        <v>4</v>
-      </c>
-      <c r="E1">
-        <v>5</v>
-      </c>
-      <c r="F1">
-        <v>6</v>
-      </c>
-      <c r="G1">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>40</v>
-      </c>
-      <c r="B2" t="s">
-        <v>41</v>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="10">
+        <v>41941</v>
       </c>
       <c r="C2" t="s">
-        <v>42</v>
-      </c>
-      <c r="D2" t="s">
-        <v>43</v>
-      </c>
-      <c r="E2" t="s">
-        <v>44</v>
-      </c>
-      <c r="F2" t="s">
-        <v>45</v>
-      </c>
-      <c r="G2" t="s">
-        <v>46</v>
-      </c>
+        <v>47</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C7" s="11"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C8" s="11"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C9" s="11"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C10" s="12"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C11" s="12"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C12" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add some links to reference
</commit_message>
<xml_diff>
--- a/Test.xlsx
+++ b/Test.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="19440" windowHeight="7935" activeTab="4"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="19440" windowHeight="7935" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Constants" sheetId="4" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="49">
   <si>
     <t>f(x,y)=x+y</t>
   </si>
@@ -162,6 +162,9 @@
   </si>
   <si>
     <t>Add color to ImageData</t>
+  </si>
+  <si>
+    <t>f(x,y)=2*x^3+y^2</t>
   </si>
 </sst>
 </file>
@@ -609,10 +612,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="C10:D10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -741,6 +744,11 @@
       </c>
       <c r="F7" t="s">
         <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -2825,7 +2833,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:C12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>

</xml_diff>